<commit_message>
#83: Implemented multiple Images to ProductDetails
</commit_message>
<xml_diff>
--- a/cintamani-next/data/products.xlsx
+++ b/cintamani-next/data/products.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oesiw\Documents\code\cintamani\cintamani-next\data\products\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oesiw\Documents\code\cintamani\cintamani-next\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
   <si>
     <t>ID</t>
   </si>
@@ -53,9 +53,6 @@
     <t>Aksobhya Kupferstatue 21cm</t>
   </si>
   <si>
-    <t>cintamani275_7</t>
-  </si>
-  <si>
     <t>Buddhas - Manjusri</t>
   </si>
   <si>
@@ -84,6 +81,24 @@
   </si>
   <si>
     <t>Beschreibung</t>
+  </si>
+  <si>
+    <t>cintamani275_7, cintamani275_7, cintamani275_7</t>
+  </si>
+  <si>
+    <t>cintamani275_7, cintamani275_7, cintamani275_8</t>
+  </si>
+  <si>
+    <t>cintamani275_7, cintamani275_7, cintamani275_9</t>
+  </si>
+  <si>
+    <t>cintamani275_7, cintamani275_7, cintamani275_10</t>
+  </si>
+  <si>
+    <t>cintamani275_7, cintamani275_7, cintamani275_11</t>
+  </si>
+  <si>
+    <t>cintamani275_7, cintamani275_7, cintamani275_12</t>
   </si>
 </sst>
 </file>
@@ -438,7 +453,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -491,10 +506,10 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="G2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -502,10 +517,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
         <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
       </c>
       <c r="D3">
         <v>649</v>
@@ -514,10 +529,10 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="G3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -525,10 +540,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D4">
         <v>250</v>
@@ -537,10 +552,10 @@
         <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="G4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -548,10 +563,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D5">
         <v>250</v>
@@ -560,10 +575,10 @@
         <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="G5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -571,10 +586,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D6">
         <v>250</v>
@@ -583,10 +598,10 @@
         <v>2</v>
       </c>
       <c r="F6" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="G6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -594,10 +609,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
         <v>17</v>
-      </c>
-      <c r="C7" t="s">
-        <v>18</v>
       </c>
       <c r="D7">
         <v>250</v>
@@ -606,10 +621,10 @@
         <v>2</v>
       </c>
       <c r="F7" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="G7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#59: Check if all images exist, before importing
</commit_message>
<xml_diff>
--- a/cintamani-next/data/products.xlsx
+++ b/cintamani-next/data/products.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
   <si>
     <t>ID</t>
   </si>
@@ -71,34 +71,13 @@
     <t>große Thangka</t>
   </si>
   <si>
-    <t>große Thangka 2</t>
-  </si>
-  <si>
-    <t>Thangkas  - klein</t>
-  </si>
-  <si>
-    <t>kleine thangka</t>
-  </si>
-  <si>
     <t>Beschreibung</t>
   </si>
   <si>
-    <t>cintamani275_7, cintamani275_7, cintamani275_7</t>
-  </si>
-  <si>
-    <t>cintamani275_7, cintamani275_7, cintamani275_8</t>
-  </si>
-  <si>
-    <t>cintamani275_7, cintamani275_7, cintamani275_9</t>
-  </si>
-  <si>
-    <t>cintamani275_7, cintamani275_7, cintamani275_10</t>
-  </si>
-  <si>
-    <t>cintamani275_7, cintamani275_7, cintamani275_11</t>
-  </si>
-  <si>
-    <t>cintamani275_7, cintamani275_7, cintamani275_12</t>
+    <t>002.jpg</t>
+  </si>
+  <si>
+    <t>001.JPG</t>
   </si>
 </sst>
 </file>
@@ -134,8 +113,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -450,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -462,7 +442,7 @@
     <col min="3" max="3" width="27" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="32.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -482,7 +462,7 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G1" t="s">
@@ -505,11 +485,11 @@
       <c r="E2">
         <v>1</v>
       </c>
-      <c r="F2" t="s">
-        <v>19</v>
+      <c r="F2" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="G2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -528,11 +508,11 @@
       <c r="E3">
         <v>1</v>
       </c>
-      <c r="F3" t="s">
-        <v>20</v>
+      <c r="F3" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="G3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -551,11 +531,11 @@
       <c r="E4">
         <v>2</v>
       </c>
-      <c r="F4" t="s">
-        <v>21</v>
+      <c r="F4" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="G4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -574,57 +554,11 @@
       <c r="E5">
         <v>2</v>
       </c>
-      <c r="F5" t="s">
-        <v>22</v>
+      <c r="F5" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="G5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" t="s">
         <v>15</v>
-      </c>
-      <c r="D6">
-        <v>250</v>
-      </c>
-      <c r="E6">
-        <v>2</v>
-      </c>
-      <c r="F6" t="s">
-        <v>23</v>
-      </c>
-      <c r="G6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7">
-        <v>250</v>
-      </c>
-      <c r="E7">
-        <v>2</v>
-      </c>
-      <c r="F7" t="s">
-        <v>24</v>
-      </c>
-      <c r="G7" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed Test data to import.
</commit_message>
<xml_diff>
--- a/cintamani-next/data/products.xlsx
+++ b/cintamani-next/data/products.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-36380" yWindow="2840" windowWidth="23040" windowHeight="9640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25720" yWindow="3300" windowWidth="23040" windowHeight="9640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="catalog_product_bearbeitet" sheetId="1" r:id="rId1"/>
@@ -2715,10 +2715,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G275"/>
+  <dimension ref="A1:G240"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A235" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G246" sqref="G246"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8225,188 +8225,7 @@
       </c>
     </row>
     <row r="240" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D240" s="1">
-        <f>SUM(D2:D239)</f>
-        <v>53282.350000000049</v>
-      </c>
-      <c r="E240">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="241" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E241">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="242" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E242">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="243" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E243">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="244" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E244">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="245" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E245">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="246" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E246">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="247" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E247">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="248" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E248">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="249" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E249">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="250" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E250">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="251" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E251">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="252" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E252">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="253" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E253">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="254" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E254">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="255" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E255">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="256" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E256">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="257" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E257">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="258" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E258">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="259" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E259">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="260" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E260">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="261" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E261">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="262" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E262">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="263" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E263">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="264" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E264">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="265" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E265">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="266" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E266">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="267" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E267">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="268" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E268">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="269" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E269">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="270" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E270">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="271" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E271">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="272" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E272">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="273" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E273">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="274" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E274">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="275" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E275">
-        <v>1</v>
-      </c>
+      <c r="D240" s="1"/>
     </row>
   </sheetData>
   <sortState ref="A218:G221">

</xml_diff>

<commit_message>
Fixed 90% of real data, renamed folders to match tabledata
</commit_message>
<xml_diff>
--- a/cintamani-next/data/products.xlsx
+++ b/cintamani-next/data/products.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-25720" yWindow="3300" windowWidth="23040" windowHeight="9640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-32460" yWindow="2160" windowWidth="23040" windowHeight="9640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="catalog_product_bearbeitet" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="959" uniqueCount="605">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="959" uniqueCount="604">
   <si>
     <t>Name</t>
   </si>
@@ -640,9 +640,6 @@
     <t>Der Türkis hat ein Gewicht von 47 Gramm, und hat eine Bohrung in der Mitte.</t>
   </si>
   <si>
-    <t>Thangkas - Big Tsagil</t>
-  </si>
-  <si>
     <t>Größe: Innen: 13x18 Außen: 40x62</t>
   </si>
   <si>
@@ -812,9 +809,6 @@
   </si>
   <si>
     <t>Die Thangka zeigt den tausendarmigen Bodhisattva Sahasrabhuja-Avalokitesvara (Sahasrabhuja Sahasranetra,jap. Senju Kanon). Der Brokat ist 50 mal 96 cm groß, das Bild ist 24,5 mal 46 cm. Vorlage für diese Thangka war der Blockdruck aus dem Buch Budddhismus Götter,Bilder und Skulpturen von Louis Frederic.</t>
-  </si>
-  <si>
-    <t>w. Bodhisattvas - Grüne Tara (Syamatara)</t>
   </si>
   <si>
     <t>Auf der Rückseite ist das Mantra_x000D_
@@ -862,9 +856,6 @@
     <t>Grüne Tara teilvergoldete Kupferstatue 8cm</t>
   </si>
   <si>
-    <t>w. Bodhisattvas - Weiße Tara (Sitatara)</t>
-  </si>
-  <si>
     <t>Dies ist eine besonders fein bearbeitete Statue mit dem Mantra der Weißen Tara_x000D_
 OM TARE TUTTATARE TURE MAMA AYUR-PUNYE PUSTIM KURU SWAHA</t>
   </si>
@@ -980,9 +971,6 @@
     <t>Maniplatte rund</t>
   </si>
   <si>
-    <t>weiteres - Räucher weiteres</t>
-  </si>
-  <si>
     <t>Räuchergefäß Löwe 20cm hoch</t>
   </si>
   <si>
@@ -1136,9 +1124,6 @@
     <t>Arapacana-Manjusri teilvergoldete Kupferstatue 22cm mit Mantra auf der Rückseite</t>
   </si>
   <si>
-    <t>w. Bodhisattvas - Usnisavijaya</t>
-  </si>
-  <si>
     <t>Usnisavijaya Kupferstatue 16cm groß</t>
   </si>
   <si>
@@ -1589,30 +1574,6 @@
     <t>TST003.JPG, TST001.JPG</t>
   </si>
   <si>
-    <t>TBT011,jpg, TBT012.JPG, TBT013,jpg, TBT014.JPG</t>
-  </si>
-  <si>
-    <t>TBT020,jpg, TBT019.JPG, TBT018,jpg</t>
-  </si>
-  <si>
-    <t>TBT021,jpg, TBT022.JPG, TBT023,jpg</t>
-  </si>
-  <si>
-    <t>TBT009,jpg, TBT025.JPG</t>
-  </si>
-  <si>
-    <t>TBT008,jpg, TBT025.JPG</t>
-  </si>
-  <si>
-    <t>TBT010,jpg, TBT025.JPG</t>
-  </si>
-  <si>
-    <t>TBT006,jpg, TBT025.JPG</t>
-  </si>
-  <si>
-    <t>TBT005,jpg, TBT003.JPG</t>
-  </si>
-  <si>
     <t>TST009.JPG, TST001.JPG</t>
   </si>
   <si>
@@ -1848,6 +1809,42 @@
   </si>
   <si>
     <t>WW008.JPG</t>
+  </si>
+  <si>
+    <t>Thangkas - big Tsagil</t>
+  </si>
+  <si>
+    <t>TBT011.JPG, TBT012.JPG, TBT013.JPG, TBT014.JPG</t>
+  </si>
+  <si>
+    <t>TBT020.jpg, TBT019.JPG, TBT018.jpg</t>
+  </si>
+  <si>
+    <t>TBT021.JPG, TBT022.JPG, TBT023.JPG</t>
+  </si>
+  <si>
+    <t>TBT009.JPG, TBT025.JPG</t>
+  </si>
+  <si>
+    <t>TBT008.JPG, TBT025.JPG</t>
+  </si>
+  <si>
+    <t>TBT010.JPG, TBT025.JPG</t>
+  </si>
+  <si>
+    <t>TBT006.JPG, TBT025.JPG</t>
+  </si>
+  <si>
+    <t>TBT005.JPG, TBT003.JPG</t>
+  </si>
+  <si>
+    <t>w Bodhisattvas - Grüne Tara (Syamatara)</t>
+  </si>
+  <si>
+    <t>w Bodhisattvas - Weiße Tara (Sitatara)</t>
+  </si>
+  <si>
+    <t>weiteres - Räucherzubehör</t>
   </si>
 </sst>
 </file>
@@ -2717,8 +2714,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G240"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A235" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G246" sqref="G246"/>
+    <sheetView tabSelected="1" topLeftCell="A206" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D217" sqref="D217"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2729,25 +2726,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="B1" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="E1" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="F1" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="G1" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -2767,7 +2764,7 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="G2" t="s">
         <v>27</v>
@@ -2790,7 +2787,7 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="G3" t="s">
         <v>4</v>
@@ -2813,7 +2810,7 @@
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="G4" t="s">
         <v>19</v>
@@ -2836,7 +2833,7 @@
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
       <c r="G5" t="s">
         <v>6</v>
@@ -2859,7 +2856,7 @@
         <v>1</v>
       </c>
       <c r="F6" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="G6" t="s">
         <v>26</v>
@@ -2882,7 +2879,7 @@
         <v>1</v>
       </c>
       <c r="F7" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="G7" t="s">
         <v>13</v>
@@ -2905,7 +2902,7 @@
         <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="G8" t="s">
         <v>17</v>
@@ -2928,7 +2925,7 @@
         <v>1</v>
       </c>
       <c r="F9" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="G9" t="s">
         <v>9</v>
@@ -2951,7 +2948,7 @@
         <v>1</v>
       </c>
       <c r="F10" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="G10" t="s">
         <v>3</v>
@@ -2974,7 +2971,7 @@
         <v>1</v>
       </c>
       <c r="F11" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="G11" t="s">
         <v>13</v>
@@ -2997,7 +2994,7 @@
         <v>1</v>
       </c>
       <c r="F12" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="G12" t="s">
         <v>13</v>
@@ -3020,7 +3017,7 @@
         <v>1</v>
       </c>
       <c r="F13" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="G13" t="s">
         <v>21</v>
@@ -3043,7 +3040,7 @@
         <v>1</v>
       </c>
       <c r="F14" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="G14" t="s">
         <v>11</v>
@@ -3066,7 +3063,7 @@
         <v>1</v>
       </c>
       <c r="F15" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="G15" t="s">
         <v>12</v>
@@ -3089,7 +3086,7 @@
         <v>1</v>
       </c>
       <c r="F16" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="G16" t="s">
         <v>2</v>
@@ -3112,7 +3109,7 @@
         <v>1</v>
       </c>
       <c r="F17" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="G17" t="s">
         <v>2</v>
@@ -3135,7 +3132,7 @@
         <v>1</v>
       </c>
       <c r="F18" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="G18" t="s">
         <v>23</v>
@@ -3158,7 +3155,7 @@
         <v>1</v>
       </c>
       <c r="F19" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="G19" t="s">
         <v>23</v>
@@ -3181,7 +3178,7 @@
         <v>1</v>
       </c>
       <c r="F20" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="G20" t="s">
         <v>18</v>
@@ -3204,7 +3201,7 @@
         <v>1</v>
       </c>
       <c r="F21" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="G21" t="s">
         <v>33</v>
@@ -3227,7 +3224,7 @@
         <v>1</v>
       </c>
       <c r="F22" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="G22" t="s">
         <v>32</v>
@@ -3250,7 +3247,7 @@
         <v>1</v>
       </c>
       <c r="F23" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="G23" t="s">
         <v>31</v>
@@ -3273,7 +3270,7 @@
         <v>1</v>
       </c>
       <c r="F24" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="G24" t="s">
         <v>29</v>
@@ -3296,7 +3293,7 @@
         <v>1</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="G25" s="3" t="s">
         <v>36</v>
@@ -3319,7 +3316,7 @@
         <v>1</v>
       </c>
       <c r="F26" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="G26" t="s">
         <v>34</v>
@@ -3342,7 +3339,7 @@
         <v>1</v>
       </c>
       <c r="F27" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="G27" t="s">
         <v>30</v>
@@ -3365,7 +3362,7 @@
         <v>1</v>
       </c>
       <c r="F28" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="G28" t="s">
         <v>42</v>
@@ -3388,7 +3385,7 @@
         <v>1</v>
       </c>
       <c r="F29" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="G29" t="s">
         <v>39</v>
@@ -3411,7 +3408,7 @@
         <v>1</v>
       </c>
       <c r="F30" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="G30" t="s">
         <v>41</v>
@@ -3434,7 +3431,7 @@
         <v>1</v>
       </c>
       <c r="F31" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="G31" t="s">
         <v>43</v>
@@ -3457,7 +3454,7 @@
         <v>1</v>
       </c>
       <c r="F32" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="G32" t="s">
         <v>40</v>
@@ -3480,7 +3477,7 @@
         <v>1</v>
       </c>
       <c r="F33" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="G33" t="s">
         <v>46</v>
@@ -3503,7 +3500,7 @@
         <v>1</v>
       </c>
       <c r="F34" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="G34" t="s">
         <v>47</v>
@@ -3526,7 +3523,7 @@
         <v>1</v>
       </c>
       <c r="F35" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="G35" t="s">
         <v>48</v>
@@ -3549,7 +3546,7 @@
         <v>1</v>
       </c>
       <c r="F36" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="G36" t="s">
         <v>45</v>
@@ -3572,7 +3569,7 @@
         <v>1</v>
       </c>
       <c r="F37" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="G37" t="s">
         <v>50</v>
@@ -3595,7 +3592,7 @@
         <v>1</v>
       </c>
       <c r="F38" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="G38" t="s">
         <v>54</v>
@@ -3618,7 +3615,7 @@
         <v>1</v>
       </c>
       <c r="F39" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="G39" t="s">
         <v>50</v>
@@ -3641,7 +3638,7 @@
         <v>1</v>
       </c>
       <c r="F40" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="G40" t="s">
         <v>55</v>
@@ -3664,7 +3661,7 @@
         <v>1</v>
       </c>
       <c r="F41" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="G41" t="s">
         <v>50</v>
@@ -3687,7 +3684,7 @@
         <v>1</v>
       </c>
       <c r="F42" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="G42" t="s">
         <v>57</v>
@@ -3710,7 +3707,7 @@
         <v>1</v>
       </c>
       <c r="F43" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="G43" t="s">
         <v>59</v>
@@ -3733,7 +3730,7 @@
         <v>1</v>
       </c>
       <c r="F44" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="G44" t="s">
         <v>61</v>
@@ -3756,7 +3753,7 @@
         <v>1</v>
       </c>
       <c r="F45" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="G45" t="s">
         <v>69</v>
@@ -3779,7 +3776,7 @@
         <v>1</v>
       </c>
       <c r="F46" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="G46" t="s">
         <v>66</v>
@@ -3802,7 +3799,7 @@
         <v>1</v>
       </c>
       <c r="F47" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="G47" t="s">
         <v>67</v>
@@ -3825,7 +3822,7 @@
         <v>1</v>
       </c>
       <c r="F48" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="G48" t="s">
         <v>68</v>
@@ -3848,7 +3845,7 @@
         <v>0</v>
       </c>
       <c r="F49" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="G49" t="s">
         <v>64</v>
@@ -3871,7 +3868,7 @@
         <v>1</v>
       </c>
       <c r="F50" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="G50" t="s">
         <v>71</v>
@@ -3894,7 +3891,7 @@
         <v>1</v>
       </c>
       <c r="F51" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="G51" t="s">
         <v>72</v>
@@ -3917,7 +3914,7 @@
         <v>1</v>
       </c>
       <c r="F52" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="G52" t="s">
         <v>78</v>
@@ -3940,7 +3937,7 @@
         <v>1</v>
       </c>
       <c r="F53" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="G53" t="s">
         <v>74</v>
@@ -3963,10 +3960,10 @@
         <v>1</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
@@ -3977,7 +3974,7 @@
         <v>73</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="D55" s="4">
         <v>399</v>
@@ -3986,7 +3983,7 @@
         <v>1</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="G55" s="3" t="s">
         <v>77</v>
@@ -4009,7 +4006,7 @@
         <v>0</v>
       </c>
       <c r="F56" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="G56" t="s">
         <v>79</v>
@@ -4032,7 +4029,7 @@
         <v>1</v>
       </c>
       <c r="F57" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="G57" t="s">
         <v>85</v>
@@ -4055,7 +4052,7 @@
         <v>1</v>
       </c>
       <c r="F58" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="G58" t="s">
         <v>84</v>
@@ -4078,7 +4075,7 @@
         <v>1</v>
       </c>
       <c r="F59" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="G59" t="s">
         <v>86</v>
@@ -4101,7 +4098,7 @@
         <v>1</v>
       </c>
       <c r="F60" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="G60" t="s">
         <v>90</v>
@@ -4124,7 +4121,7 @@
         <v>1</v>
       </c>
       <c r="F61" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="G61" t="s">
         <v>88</v>
@@ -4138,7 +4135,7 @@
         <v>81</v>
       </c>
       <c r="C62" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="D62" s="1">
         <v>299</v>
@@ -4147,10 +4144,10 @@
         <v>1</v>
       </c>
       <c r="F62" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="G62" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
@@ -4170,7 +4167,7 @@
         <v>0</v>
       </c>
       <c r="F63" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="G63" t="s">
         <v>87</v>
@@ -4193,7 +4190,7 @@
         <v>1</v>
       </c>
       <c r="F64" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="G64" t="s">
         <v>82</v>
@@ -4216,7 +4213,7 @@
         <v>1</v>
       </c>
       <c r="F65" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="G65" t="s">
         <v>92</v>
@@ -4239,7 +4236,7 @@
         <v>1</v>
       </c>
       <c r="F66" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="G66" s="5" t="s">
         <v>95</v>
@@ -4262,7 +4259,7 @@
         <v>1</v>
       </c>
       <c r="F67" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="G67" t="s">
         <v>102</v>
@@ -4285,7 +4282,7 @@
         <v>1</v>
       </c>
       <c r="F68" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="G68" t="s">
         <v>98</v>
@@ -4308,7 +4305,7 @@
         <v>1</v>
       </c>
       <c r="F69" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
       <c r="G69" t="s">
         <v>99</v>
@@ -4331,7 +4328,7 @@
         <v>1</v>
       </c>
       <c r="F70" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
       <c r="G70" t="s">
         <v>100</v>
@@ -4342,7 +4339,7 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="C71" t="s">
         <v>119</v>
@@ -4354,7 +4351,7 @@
         <v>1</v>
       </c>
       <c r="F71" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
       <c r="G71" t="s">
         <v>118</v>
@@ -4365,7 +4362,7 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="C72" t="s">
         <v>121</v>
@@ -4377,7 +4374,7 @@
         <v>1</v>
       </c>
       <c r="F72" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="G72" t="s">
         <v>120</v>
@@ -4388,7 +4385,7 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="C73" t="s">
         <v>109</v>
@@ -4400,7 +4397,7 @@
         <v>1</v>
       </c>
       <c r="F73" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="G73" t="s">
         <v>108</v>
@@ -4411,7 +4408,7 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="C74" t="s">
         <v>111</v>
@@ -4423,7 +4420,7 @@
         <v>1</v>
       </c>
       <c r="F74" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="G74" t="s">
         <v>110</v>
@@ -4434,7 +4431,7 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="C75" t="s">
         <v>113</v>
@@ -4446,7 +4443,7 @@
         <v>1</v>
       </c>
       <c r="F75" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="G75" t="s">
         <v>112</v>
@@ -4457,7 +4454,7 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="C76" t="s">
         <v>115</v>
@@ -4469,7 +4466,7 @@
         <v>1</v>
       </c>
       <c r="F76" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
       <c r="G76" t="s">
         <v>114</v>
@@ -4480,7 +4477,7 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="C77" t="s">
         <v>117</v>
@@ -4492,7 +4489,7 @@
         <v>1</v>
       </c>
       <c r="F77" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="G77" t="s">
         <v>116</v>
@@ -4503,7 +4500,7 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="C78" t="s">
         <v>105</v>
@@ -4515,7 +4512,7 @@
         <v>1</v>
       </c>
       <c r="F78" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
       <c r="G78" t="s">
         <v>103</v>
@@ -4526,7 +4523,7 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="C79" t="s">
         <v>104</v>
@@ -4538,7 +4535,7 @@
         <v>1</v>
       </c>
       <c r="F79" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
       <c r="G79" t="s">
         <v>103</v>
@@ -4549,7 +4546,7 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="C80" t="s">
         <v>106</v>
@@ -4561,7 +4558,7 @@
         <v>1</v>
       </c>
       <c r="F80" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
       <c r="G80" t="s">
         <v>103</v>
@@ -4572,7 +4569,7 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="C81" t="s">
         <v>107</v>
@@ -4584,7 +4581,7 @@
         <v>1</v>
       </c>
       <c r="F81" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
       <c r="G81" t="s">
         <v>103</v>
@@ -4607,7 +4604,7 @@
         <v>1</v>
       </c>
       <c r="F82" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="G82" t="s">
         <v>129</v>
@@ -4630,7 +4627,7 @@
         <v>1</v>
       </c>
       <c r="F83" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
       <c r="G83" t="s">
         <v>137</v>
@@ -4653,7 +4650,7 @@
         <v>1</v>
       </c>
       <c r="F84" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
       <c r="G84" t="s">
         <v>136</v>
@@ -4676,7 +4673,7 @@
         <v>1</v>
       </c>
       <c r="F85" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
       <c r="G85" t="s">
         <v>133</v>
@@ -4699,7 +4696,7 @@
         <v>1</v>
       </c>
       <c r="F86" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
       <c r="G86" t="s">
         <v>130</v>
@@ -4722,7 +4719,7 @@
         <v>1</v>
       </c>
       <c r="F87" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
       <c r="G87" t="s">
         <v>132</v>
@@ -4745,10 +4742,10 @@
         <v>1</v>
       </c>
       <c r="F88" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
       <c r="G88" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
@@ -4768,7 +4765,7 @@
         <v>1</v>
       </c>
       <c r="F89" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
       <c r="G89" t="s">
         <v>138</v>
@@ -4791,7 +4788,7 @@
         <v>1</v>
       </c>
       <c r="F90" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="G90" t="s">
         <v>123</v>
@@ -4814,7 +4811,7 @@
         <v>0</v>
       </c>
       <c r="F91" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
       <c r="G91" t="s">
         <v>127</v>
@@ -4828,7 +4825,7 @@
         <v>122</v>
       </c>
       <c r="C92" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="D92" s="1">
         <v>299</v>
@@ -4837,10 +4834,10 @@
         <v>1</v>
       </c>
       <c r="F92" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="G92" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.2">
@@ -4851,7 +4848,7 @@
         <v>122</v>
       </c>
       <c r="C93" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="D93" s="1">
         <v>399</v>
@@ -4860,10 +4857,10 @@
         <v>1</v>
       </c>
       <c r="F93" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="G93" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
@@ -4883,7 +4880,7 @@
         <v>1</v>
       </c>
       <c r="F94" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="G94" t="s">
         <v>125</v>
@@ -4906,7 +4903,7 @@
         <v>1</v>
       </c>
       <c r="F95" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
       <c r="G95" t="s">
         <v>134</v>
@@ -4929,7 +4926,7 @@
         <v>1</v>
       </c>
       <c r="F96" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
       <c r="G96" t="s">
         <v>144</v>
@@ -4943,7 +4940,7 @@
         <v>140</v>
       </c>
       <c r="C97" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="D97" s="1">
         <v>59</v>
@@ -4952,10 +4949,10 @@
         <v>1</v>
       </c>
       <c r="F97" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
       <c r="G97" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.2">
@@ -4975,7 +4972,7 @@
         <v>1</v>
       </c>
       <c r="F98" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="G98" t="s">
         <v>143</v>
@@ -4998,7 +4995,7 @@
         <v>1</v>
       </c>
       <c r="F99" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="G99" t="s">
         <v>145</v>
@@ -5012,7 +5009,7 @@
         <v>140</v>
       </c>
       <c r="C100" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="D100" s="1">
         <v>179</v>
@@ -5021,10 +5018,10 @@
         <v>1</v>
       </c>
       <c r="F100" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="G100" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.2">
@@ -5044,7 +5041,7 @@
         <v>1</v>
       </c>
       <c r="F101" t="s">
-        <v>475</v>
+        <v>470</v>
       </c>
       <c r="G101" s="5" t="s">
         <v>141</v>
@@ -5058,7 +5055,7 @@
         <v>140</v>
       </c>
       <c r="C102" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="D102" s="1">
         <v>399</v>
@@ -5067,10 +5064,10 @@
         <v>1</v>
       </c>
       <c r="F102" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
       <c r="G102" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.2">
@@ -5090,7 +5087,7 @@
         <v>1</v>
       </c>
       <c r="F103" t="s">
-        <v>477</v>
+        <v>472</v>
       </c>
       <c r="G103" s="5" t="s">
         <v>150</v>
@@ -5113,7 +5110,7 @@
         <v>1</v>
       </c>
       <c r="F104" t="s">
-        <v>478</v>
+        <v>473</v>
       </c>
       <c r="G104" t="s">
         <v>146</v>
@@ -5136,7 +5133,7 @@
         <v>1</v>
       </c>
       <c r="F105" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
       <c r="G105" s="5" t="s">
         <v>147</v>
@@ -5159,7 +5156,7 @@
         <v>1</v>
       </c>
       <c r="F106" t="s">
-        <v>480</v>
+        <v>475</v>
       </c>
       <c r="G106" t="s">
         <v>170</v>
@@ -5182,7 +5179,7 @@
         <v>1</v>
       </c>
       <c r="F107" t="s">
-        <v>481</v>
+        <v>476</v>
       </c>
       <c r="G107" t="s">
         <v>170</v>
@@ -5205,7 +5202,7 @@
         <v>1</v>
       </c>
       <c r="F108" t="s">
-        <v>482</v>
+        <v>477</v>
       </c>
       <c r="G108" t="s">
         <v>170</v>
@@ -5228,7 +5225,7 @@
         <v>1</v>
       </c>
       <c r="F109" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
       <c r="G109" t="s">
         <v>170</v>
@@ -5251,7 +5248,7 @@
         <v>1</v>
       </c>
       <c r="F110" t="s">
-        <v>484</v>
+        <v>479</v>
       </c>
       <c r="G110" t="s">
         <v>170</v>
@@ -5274,7 +5271,7 @@
         <v>1</v>
       </c>
       <c r="F111" t="s">
-        <v>485</v>
+        <v>480</v>
       </c>
       <c r="G111" t="s">
         <v>170</v>
@@ -5297,7 +5294,7 @@
         <v>1</v>
       </c>
       <c r="F112" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="G112" t="s">
         <v>153</v>
@@ -5320,7 +5317,7 @@
         <v>1</v>
       </c>
       <c r="F113" t="s">
-        <v>487</v>
+        <v>482</v>
       </c>
       <c r="G113" t="s">
         <v>178</v>
@@ -5343,7 +5340,7 @@
         <v>1</v>
       </c>
       <c r="F114" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
       <c r="G114" t="s">
         <v>165</v>
@@ -5366,7 +5363,7 @@
         <v>1</v>
       </c>
       <c r="F115" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
       <c r="G115" t="s">
         <v>165</v>
@@ -5389,7 +5386,7 @@
         <v>1</v>
       </c>
       <c r="F116" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
       <c r="G116" t="s">
         <v>168</v>
@@ -5412,7 +5409,7 @@
         <v>1</v>
       </c>
       <c r="F117" t="s">
-        <v>491</v>
+        <v>486</v>
       </c>
       <c r="G117" t="s">
         <v>165</v>
@@ -5435,7 +5432,7 @@
         <v>1</v>
       </c>
       <c r="F118" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="G118" t="s">
         <v>155</v>
@@ -5458,7 +5455,7 @@
         <v>1</v>
       </c>
       <c r="F119" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
       <c r="G119" t="s">
         <v>164</v>
@@ -5481,7 +5478,7 @@
         <v>1</v>
       </c>
       <c r="F120" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
       <c r="G120" t="s">
         <v>170</v>
@@ -5495,7 +5492,7 @@
         <v>152</v>
       </c>
       <c r="C121" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="D121" s="1">
         <v>9.9</v>
@@ -5504,7 +5501,7 @@
         <v>1</v>
       </c>
       <c r="F121" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
       <c r="G121" t="s">
         <v>170</v>
@@ -5527,7 +5524,7 @@
         <v>1</v>
       </c>
       <c r="F122" t="s">
-        <v>495</v>
+        <v>490</v>
       </c>
       <c r="G122" t="s">
         <v>159</v>
@@ -5550,7 +5547,7 @@
         <v>1</v>
       </c>
       <c r="F123" t="s">
-        <v>495</v>
+        <v>490</v>
       </c>
       <c r="G123" t="s">
         <v>157</v>
@@ -5573,7 +5570,7 @@
         <v>1</v>
       </c>
       <c r="F124" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
       <c r="G124" t="s">
         <v>161</v>
@@ -5596,7 +5593,7 @@
         <v>1</v>
       </c>
       <c r="F125" t="s">
-        <v>497</v>
+        <v>492</v>
       </c>
       <c r="G125" t="s">
         <v>162</v>
@@ -5619,7 +5616,7 @@
         <v>1</v>
       </c>
       <c r="F126" t="s">
-        <v>498</v>
+        <v>493</v>
       </c>
       <c r="G126" t="s">
         <v>163</v>
@@ -5633,7 +5630,7 @@
         <v>179</v>
       </c>
       <c r="C127" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="D127" s="1">
         <v>9.9</v>
@@ -5642,7 +5639,7 @@
         <v>1</v>
       </c>
       <c r="F127" t="s">
-        <v>499</v>
+        <v>494</v>
       </c>
       <c r="G127" t="s">
         <v>180</v>
@@ -5665,7 +5662,7 @@
         <v>1</v>
       </c>
       <c r="F128" t="s">
-        <v>500</v>
+        <v>495</v>
       </c>
       <c r="G128" t="s">
         <v>180</v>
@@ -5679,7 +5676,7 @@
         <v>179</v>
       </c>
       <c r="C129" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="D129" s="1">
         <v>10</v>
@@ -5688,7 +5685,7 @@
         <v>1</v>
       </c>
       <c r="F129" t="s">
-        <v>501</v>
+        <v>496</v>
       </c>
       <c r="G129" t="s">
         <v>180</v>
@@ -5711,7 +5708,7 @@
         <v>1</v>
       </c>
       <c r="F130" t="s">
-        <v>502</v>
+        <v>497</v>
       </c>
       <c r="G130" t="s">
         <v>180</v>
@@ -5734,7 +5731,7 @@
         <v>1</v>
       </c>
       <c r="F131" t="s">
-        <v>503</v>
+        <v>498</v>
       </c>
       <c r="G131" t="s">
         <v>180</v>
@@ -5757,7 +5754,7 @@
         <v>1</v>
       </c>
       <c r="F132" t="s">
-        <v>504</v>
+        <v>499</v>
       </c>
       <c r="G132" t="s">
         <v>180</v>
@@ -5780,7 +5777,7 @@
         <v>1</v>
       </c>
       <c r="F133" t="s">
-        <v>505</v>
+        <v>500</v>
       </c>
       <c r="G133" t="s">
         <v>201</v>
@@ -5803,7 +5800,7 @@
         <v>1</v>
       </c>
       <c r="F134" t="s">
-        <v>506</v>
+        <v>501</v>
       </c>
       <c r="G134" t="s">
         <v>180</v>
@@ -5826,7 +5823,7 @@
         <v>1</v>
       </c>
       <c r="F135" t="s">
-        <v>504</v>
+        <v>499</v>
       </c>
       <c r="G135" t="s">
         <v>180</v>
@@ -5849,7 +5846,7 @@
         <v>1</v>
       </c>
       <c r="F136" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
       <c r="G136" t="s">
         <v>180</v>
@@ -5872,7 +5869,7 @@
         <v>1</v>
       </c>
       <c r="F137" t="s">
-        <v>508</v>
+        <v>503</v>
       </c>
       <c r="G137" t="s">
         <v>190</v>
@@ -5895,7 +5892,7 @@
         <v>1</v>
       </c>
       <c r="F138" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="G138" t="s">
         <v>203</v>
@@ -5918,7 +5915,7 @@
         <v>1</v>
       </c>
       <c r="F139" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
       <c r="G139" t="s">
         <v>180</v>
@@ -5941,7 +5938,7 @@
         <v>1</v>
       </c>
       <c r="F140" t="s">
-        <v>511</v>
+        <v>506</v>
       </c>
       <c r="G140" t="s">
         <v>199</v>
@@ -5964,7 +5961,7 @@
         <v>1</v>
       </c>
       <c r="F141" t="s">
-        <v>512</v>
+        <v>507</v>
       </c>
       <c r="G141" t="s">
         <v>180</v>
@@ -5987,7 +5984,7 @@
         <v>1</v>
       </c>
       <c r="F142" t="s">
-        <v>513</v>
+        <v>508</v>
       </c>
       <c r="G142" t="s">
         <v>180</v>
@@ -6010,7 +6007,7 @@
         <v>1</v>
       </c>
       <c r="F143" t="s">
-        <v>514</v>
+        <v>509</v>
       </c>
       <c r="G143" t="s">
         <v>195</v>
@@ -6033,7 +6030,7 @@
         <v>1</v>
       </c>
       <c r="F144" t="s">
-        <v>515</v>
+        <v>510</v>
       </c>
       <c r="G144" t="s">
         <v>193</v>
@@ -6056,7 +6053,7 @@
         <v>1</v>
       </c>
       <c r="F145" t="s">
-        <v>516</v>
+        <v>511</v>
       </c>
       <c r="G145" t="s">
         <v>193</v>
@@ -6067,10 +6064,10 @@
         <v>145</v>
       </c>
       <c r="B146" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C146" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D146" s="1">
         <v>49.9</v>
@@ -6079,10 +6076,10 @@
         <v>1</v>
       </c>
       <c r="F146" t="s">
-        <v>517</v>
+        <v>512</v>
       </c>
       <c r="G146" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.2">
@@ -6090,10 +6087,10 @@
         <v>146</v>
       </c>
       <c r="B147" t="s">
-        <v>204</v>
+        <v>592</v>
       </c>
       <c r="C147" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D147" s="1">
         <v>89</v>
@@ -6102,10 +6099,10 @@
         <v>1</v>
       </c>
       <c r="F147" t="s">
-        <v>518</v>
+        <v>593</v>
       </c>
       <c r="G147" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.2">
@@ -6113,10 +6110,10 @@
         <v>147</v>
       </c>
       <c r="B148" t="s">
-        <v>204</v>
+        <v>592</v>
       </c>
       <c r="C148" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D148" s="1">
         <v>89</v>
@@ -6125,10 +6122,10 @@
         <v>1</v>
       </c>
       <c r="F148" t="s">
-        <v>519</v>
+        <v>594</v>
       </c>
       <c r="G148" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.2">
@@ -6136,10 +6133,10 @@
         <v>148</v>
       </c>
       <c r="B149" t="s">
-        <v>204</v>
+        <v>592</v>
       </c>
       <c r="C149" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D149" s="1">
         <v>89</v>
@@ -6148,10 +6145,10 @@
         <v>1</v>
       </c>
       <c r="F149" t="s">
-        <v>520</v>
+        <v>595</v>
       </c>
       <c r="G149" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.2">
@@ -6159,10 +6156,10 @@
         <v>149</v>
       </c>
       <c r="B150" t="s">
-        <v>204</v>
+        <v>592</v>
       </c>
       <c r="C150" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D150" s="1">
         <v>99</v>
@@ -6171,10 +6168,10 @@
         <v>1</v>
       </c>
       <c r="F150" t="s">
-        <v>521</v>
+        <v>596</v>
       </c>
       <c r="G150" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.2">
@@ -6182,10 +6179,10 @@
         <v>150</v>
       </c>
       <c r="B151" t="s">
-        <v>204</v>
+        <v>592</v>
       </c>
       <c r="C151" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D151" s="1">
         <v>99</v>
@@ -6194,10 +6191,10 @@
         <v>1</v>
       </c>
       <c r="F151" t="s">
-        <v>522</v>
+        <v>597</v>
       </c>
       <c r="G151" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.2">
@@ -6205,10 +6202,10 @@
         <v>151</v>
       </c>
       <c r="B152" t="s">
-        <v>204</v>
+        <v>592</v>
       </c>
       <c r="C152" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D152" s="1">
         <v>99</v>
@@ -6217,10 +6214,10 @@
         <v>1</v>
       </c>
       <c r="F152" t="s">
-        <v>523</v>
+        <v>598</v>
       </c>
       <c r="G152" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.2">
@@ -6228,10 +6225,10 @@
         <v>152</v>
       </c>
       <c r="B153" t="s">
-        <v>204</v>
+        <v>592</v>
       </c>
       <c r="C153" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D153" s="1">
         <v>99</v>
@@ -6240,10 +6237,10 @@
         <v>1</v>
       </c>
       <c r="F153" t="s">
-        <v>524</v>
+        <v>599</v>
       </c>
       <c r="G153" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.2">
@@ -6251,10 +6248,10 @@
         <v>153</v>
       </c>
       <c r="B154" t="s">
-        <v>204</v>
+        <v>592</v>
       </c>
       <c r="C154" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D154" s="1">
         <v>179</v>
@@ -6263,10 +6260,10 @@
         <v>1</v>
       </c>
       <c r="F154" t="s">
-        <v>525</v>
+        <v>600</v>
       </c>
       <c r="G154" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.2">
@@ -6274,10 +6271,10 @@
         <v>154</v>
       </c>
       <c r="B155" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C155" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D155" s="1">
         <v>49.9</v>
@@ -6286,10 +6283,10 @@
         <v>1</v>
       </c>
       <c r="F155" t="s">
-        <v>526</v>
+        <v>513</v>
       </c>
       <c r="G155" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.2">
@@ -6297,10 +6294,10 @@
         <v>155</v>
       </c>
       <c r="B156" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C156" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D156" s="1">
         <v>49.9</v>
@@ -6309,10 +6306,10 @@
         <v>1</v>
       </c>
       <c r="F156" t="s">
-        <v>527</v>
+        <v>514</v>
       </c>
       <c r="G156" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.2">
@@ -6320,10 +6317,10 @@
         <v>156</v>
       </c>
       <c r="B157" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C157" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D157" s="1">
         <v>49.9</v>
@@ -6332,10 +6329,10 @@
         <v>1</v>
       </c>
       <c r="F157" t="s">
-        <v>528</v>
+        <v>515</v>
       </c>
       <c r="G157" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.2">
@@ -6343,10 +6340,10 @@
         <v>157</v>
       </c>
       <c r="B158" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C158" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D158" s="1">
         <v>49.9</v>
@@ -6355,10 +6352,10 @@
         <v>1</v>
       </c>
       <c r="F158" t="s">
-        <v>529</v>
+        <v>516</v>
       </c>
       <c r="G158" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.2">
@@ -6366,10 +6363,10 @@
         <v>158</v>
       </c>
       <c r="B159" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C159" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D159" s="1">
         <v>49.9</v>
@@ -6378,10 +6375,10 @@
         <v>1</v>
       </c>
       <c r="F159" t="s">
-        <v>530</v>
+        <v>517</v>
       </c>
       <c r="G159" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.2">
@@ -6389,10 +6386,10 @@
         <v>159</v>
       </c>
       <c r="B160" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C160" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D160" s="1">
         <v>49.9</v>
@@ -6401,10 +6398,10 @@
         <v>1</v>
       </c>
       <c r="F160" t="s">
-        <v>531</v>
+        <v>518</v>
       </c>
       <c r="G160" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.2">
@@ -6412,10 +6409,10 @@
         <v>160</v>
       </c>
       <c r="B161" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C161" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D161" s="1">
         <v>49.9</v>
@@ -6424,10 +6421,10 @@
         <v>1</v>
       </c>
       <c r="F161" t="s">
-        <v>532</v>
+        <v>519</v>
       </c>
       <c r="G161" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.2">
@@ -6435,10 +6432,10 @@
         <v>161</v>
       </c>
       <c r="B162" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C162" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D162" s="1">
         <v>49.9</v>
@@ -6447,10 +6444,10 @@
         <v>1</v>
       </c>
       <c r="F162" t="s">
-        <v>533</v>
+        <v>520</v>
       </c>
       <c r="G162" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.2">
@@ -6458,10 +6455,10 @@
         <v>162</v>
       </c>
       <c r="B163" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C163" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D163" s="1">
         <v>49.9</v>
@@ -6470,10 +6467,10 @@
         <v>1</v>
       </c>
       <c r="F163" t="s">
-        <v>534</v>
+        <v>521</v>
       </c>
       <c r="G163" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.2">
@@ -6481,10 +6478,10 @@
         <v>163</v>
       </c>
       <c r="B164" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C164" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D164" s="1">
         <v>199</v>
@@ -6493,10 +6490,10 @@
         <v>1</v>
       </c>
       <c r="F164" t="s">
-        <v>535</v>
+        <v>522</v>
       </c>
       <c r="G164" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.2">
@@ -6504,10 +6501,10 @@
         <v>164</v>
       </c>
       <c r="B165" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C165" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D165" s="1">
         <v>199</v>
@@ -6516,10 +6513,10 @@
         <v>1</v>
       </c>
       <c r="F165" t="s">
-        <v>536</v>
+        <v>523</v>
       </c>
       <c r="G165" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.2">
@@ -6527,10 +6524,10 @@
         <v>165</v>
       </c>
       <c r="B166" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C166" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D166" s="1">
         <v>199</v>
@@ -6539,10 +6536,10 @@
         <v>1</v>
       </c>
       <c r="F166" t="s">
-        <v>537</v>
+        <v>524</v>
       </c>
       <c r="G166" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.2">
@@ -6550,10 +6547,10 @@
         <v>166</v>
       </c>
       <c r="B167" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C167" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D167" s="1">
         <v>199</v>
@@ -6562,10 +6559,10 @@
         <v>1</v>
       </c>
       <c r="F167" t="s">
-        <v>538</v>
+        <v>525</v>
       </c>
       <c r="G167" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.2">
@@ -6573,10 +6570,10 @@
         <v>167</v>
       </c>
       <c r="B168" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C168" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D168" s="1">
         <v>249</v>
@@ -6585,10 +6582,10 @@
         <v>1</v>
       </c>
       <c r="F168" t="s">
-        <v>539</v>
+        <v>526</v>
       </c>
       <c r="G168" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.2">
@@ -6596,10 +6593,10 @@
         <v>168</v>
       </c>
       <c r="B169" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C169" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D169" s="1">
         <v>249</v>
@@ -6608,10 +6605,10 @@
         <v>1</v>
       </c>
       <c r="F169" t="s">
-        <v>540</v>
+        <v>527</v>
       </c>
       <c r="G169" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.2">
@@ -6619,10 +6616,10 @@
         <v>169</v>
       </c>
       <c r="B170" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C170" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D170" s="1">
         <v>249</v>
@@ -6631,10 +6628,10 @@
         <v>1</v>
       </c>
       <c r="F170" t="s">
-        <v>541</v>
+        <v>528</v>
       </c>
       <c r="G170" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.2">
@@ -6642,10 +6639,10 @@
         <v>170</v>
       </c>
       <c r="B171" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C171" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D171" s="1">
         <v>399</v>
@@ -6654,10 +6651,10 @@
         <v>1</v>
       </c>
       <c r="F171" t="s">
-        <v>542</v>
+        <v>529</v>
       </c>
       <c r="G171" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.2">
@@ -6665,10 +6662,10 @@
         <v>171</v>
       </c>
       <c r="B172" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C172" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D172" s="4">
         <v>399</v>
@@ -6677,10 +6674,10 @@
         <v>1</v>
       </c>
       <c r="F172" s="3" t="s">
-        <v>543</v>
+        <v>530</v>
       </c>
       <c r="G172" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.2">
@@ -6688,10 +6685,10 @@
         <v>172</v>
       </c>
       <c r="B173" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C173" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D173" s="4">
         <v>399</v>
@@ -6700,10 +6697,10 @@
         <v>1</v>
       </c>
       <c r="F173" s="3" t="s">
-        <v>544</v>
+        <v>531</v>
       </c>
       <c r="G173" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.2">
@@ -6711,10 +6708,10 @@
         <v>173</v>
       </c>
       <c r="B174" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C174" s="3" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="D174" s="4">
         <v>399</v>
@@ -6723,10 +6720,10 @@
         <v>1</v>
       </c>
       <c r="F174" s="3" t="s">
-        <v>545</v>
+        <v>532</v>
       </c>
       <c r="G174" s="3" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.2">
@@ -6734,10 +6731,10 @@
         <v>174</v>
       </c>
       <c r="B175" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C175" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D175" s="1">
         <v>499</v>
@@ -6746,10 +6743,10 @@
         <v>1</v>
       </c>
       <c r="F175" t="s">
-        <v>546</v>
+        <v>533</v>
       </c>
       <c r="G175" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.2">
@@ -6757,10 +6754,10 @@
         <v>175</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C176" s="3" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="D176" s="4">
         <v>499</v>
@@ -6769,10 +6766,10 @@
         <v>1</v>
       </c>
       <c r="F176" s="3" t="s">
-        <v>547</v>
+        <v>534</v>
       </c>
       <c r="G176" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="177" spans="1:7" x14ac:dyDescent="0.2">
@@ -6780,10 +6777,10 @@
         <v>176</v>
       </c>
       <c r="B177" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C177" s="3" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="D177" s="4">
         <v>799</v>
@@ -6792,10 +6789,10 @@
         <v>1</v>
       </c>
       <c r="F177" s="3" t="s">
-        <v>548</v>
+        <v>535</v>
       </c>
       <c r="G177" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="178" spans="1:7" x14ac:dyDescent="0.2">
@@ -6803,10 +6800,10 @@
         <v>177</v>
       </c>
       <c r="B178" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C178" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D178" s="1">
         <v>999</v>
@@ -6815,10 +6812,10 @@
         <v>1</v>
       </c>
       <c r="F178" t="s">
-        <v>549</v>
+        <v>536</v>
       </c>
       <c r="G178" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.2">
@@ -6826,10 +6823,10 @@
         <v>178</v>
       </c>
       <c r="B179" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C179" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D179" s="1">
         <v>999</v>
@@ -6838,10 +6835,10 @@
         <v>1</v>
       </c>
       <c r="F179" t="s">
-        <v>550</v>
+        <v>537</v>
       </c>
       <c r="G179" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="180" spans="1:7" x14ac:dyDescent="0.2">
@@ -6849,10 +6846,10 @@
         <v>179</v>
       </c>
       <c r="B180" t="s">
-        <v>367</v>
+        <v>94</v>
       </c>
       <c r="C180" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="D180" s="1">
         <v>499</v>
@@ -6861,10 +6858,10 @@
         <v>1</v>
       </c>
       <c r="F180" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="G180" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.2">
@@ -6872,10 +6869,10 @@
         <v>180</v>
       </c>
       <c r="B181" t="s">
-        <v>367</v>
+        <v>94</v>
       </c>
       <c r="C181" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D181" s="1">
         <v>19.5</v>
@@ -6884,10 +6881,10 @@
         <v>1</v>
       </c>
       <c r="F181" t="s">
-        <v>551</v>
+        <v>538</v>
       </c>
       <c r="G181" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.2">
@@ -6895,10 +6892,10 @@
         <v>181</v>
       </c>
       <c r="B182" t="s">
-        <v>262</v>
+        <v>601</v>
       </c>
       <c r="C182" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D182" s="1">
         <v>59</v>
@@ -6907,10 +6904,10 @@
         <v>1</v>
       </c>
       <c r="F182" t="s">
-        <v>552</v>
+        <v>539</v>
       </c>
       <c r="G182" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="183" spans="1:7" x14ac:dyDescent="0.2">
@@ -6918,10 +6915,10 @@
         <v>182</v>
       </c>
       <c r="B183" t="s">
-        <v>262</v>
+        <v>601</v>
       </c>
       <c r="C183" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D183" s="1">
         <v>69</v>
@@ -6930,10 +6927,10 @@
         <v>1</v>
       </c>
       <c r="F183" t="s">
-        <v>553</v>
+        <v>540</v>
       </c>
       <c r="G183" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="184" spans="1:7" x14ac:dyDescent="0.2">
@@ -6941,10 +6938,10 @@
         <v>183</v>
       </c>
       <c r="B184" t="s">
-        <v>262</v>
+        <v>601</v>
       </c>
       <c r="C184" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D184" s="1">
         <v>99</v>
@@ -6953,10 +6950,10 @@
         <v>1</v>
       </c>
       <c r="F184" t="s">
-        <v>554</v>
+        <v>541</v>
       </c>
       <c r="G184" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="185" spans="1:7" x14ac:dyDescent="0.2">
@@ -6964,10 +6961,10 @@
         <v>184</v>
       </c>
       <c r="B185" t="s">
-        <v>262</v>
+        <v>601</v>
       </c>
       <c r="C185" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D185" s="1">
         <v>229</v>
@@ -6976,10 +6973,10 @@
         <v>1</v>
       </c>
       <c r="F185" t="s">
-        <v>555</v>
+        <v>542</v>
       </c>
       <c r="G185" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="186" spans="1:7" x14ac:dyDescent="0.2">
@@ -6987,10 +6984,10 @@
         <v>185</v>
       </c>
       <c r="B186" t="s">
-        <v>262</v>
+        <v>601</v>
       </c>
       <c r="C186" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D186" s="1">
         <v>269</v>
@@ -6999,10 +6996,10 @@
         <v>0</v>
       </c>
       <c r="F186" t="s">
-        <v>556</v>
+        <v>543</v>
       </c>
       <c r="G186" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="187" spans="1:7" x14ac:dyDescent="0.2">
@@ -7010,10 +7007,10 @@
         <v>186</v>
       </c>
       <c r="B187" t="s">
-        <v>262</v>
+        <v>601</v>
       </c>
       <c r="C187" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D187" s="1">
         <v>269</v>
@@ -7022,10 +7019,10 @@
         <v>1</v>
       </c>
       <c r="F187" t="s">
-        <v>557</v>
+        <v>544</v>
       </c>
       <c r="G187" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="188" spans="1:7" x14ac:dyDescent="0.2">
@@ -7033,10 +7030,10 @@
         <v>187</v>
       </c>
       <c r="B188" t="s">
-        <v>262</v>
+        <v>601</v>
       </c>
       <c r="C188" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D188" s="1">
         <v>399</v>
@@ -7045,10 +7042,10 @@
         <v>1</v>
       </c>
       <c r="F188" t="s">
-        <v>558</v>
+        <v>545</v>
       </c>
       <c r="G188" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="189" spans="1:7" x14ac:dyDescent="0.2">
@@ -7056,10 +7053,10 @@
         <v>188</v>
       </c>
       <c r="B189" t="s">
-        <v>262</v>
+        <v>601</v>
       </c>
       <c r="C189" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D189" s="1">
         <v>799</v>
@@ -7068,10 +7065,10 @@
         <v>1</v>
       </c>
       <c r="F189" t="s">
-        <v>559</v>
+        <v>546</v>
       </c>
       <c r="G189" s="5" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="190" spans="1:7" x14ac:dyDescent="0.2">
@@ -7079,10 +7076,10 @@
         <v>189</v>
       </c>
       <c r="B190" t="s">
-        <v>262</v>
+        <v>601</v>
       </c>
       <c r="C190" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D190" s="1">
         <v>999</v>
@@ -7091,10 +7088,10 @@
         <v>1</v>
       </c>
       <c r="F190" t="s">
-        <v>560</v>
+        <v>547</v>
       </c>
       <c r="G190" s="5" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="191" spans="1:7" x14ac:dyDescent="0.2">
@@ -7102,10 +7099,10 @@
         <v>190</v>
       </c>
       <c r="B191" t="s">
+        <v>601</v>
+      </c>
+      <c r="C191" t="s">
         <v>262</v>
-      </c>
-      <c r="C191" t="s">
-        <v>264</v>
       </c>
       <c r="D191" s="1">
         <v>1299</v>
@@ -7114,10 +7111,10 @@
         <v>1</v>
       </c>
       <c r="F191" t="s">
-        <v>561</v>
+        <v>548</v>
       </c>
       <c r="G191" s="5" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="192" spans="1:7" x14ac:dyDescent="0.2">
@@ -7125,10 +7122,10 @@
         <v>191</v>
       </c>
       <c r="B192" t="s">
-        <v>262</v>
+        <v>601</v>
       </c>
       <c r="C192" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D192" s="1">
         <v>1399</v>
@@ -7137,10 +7134,10 @@
         <v>1</v>
       </c>
       <c r="F192" t="s">
-        <v>562</v>
+        <v>549</v>
       </c>
       <c r="G192" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="193" spans="1:7" x14ac:dyDescent="0.2">
@@ -7148,10 +7145,10 @@
         <v>192</v>
       </c>
       <c r="B193" t="s">
-        <v>277</v>
+        <v>602</v>
       </c>
       <c r="C193" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="D193" s="1">
         <v>19.5</v>
@@ -7160,10 +7157,10 @@
         <v>1</v>
       </c>
       <c r="F193" t="s">
-        <v>563</v>
+        <v>550</v>
       </c>
       <c r="G193" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="194" spans="1:7" x14ac:dyDescent="0.2">
@@ -7171,10 +7168,10 @@
         <v>193</v>
       </c>
       <c r="B194" t="s">
-        <v>277</v>
+        <v>602</v>
       </c>
       <c r="C194" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="D194" s="1">
         <v>59</v>
@@ -7183,10 +7180,10 @@
         <v>1</v>
       </c>
       <c r="F194" t="s">
-        <v>564</v>
+        <v>551</v>
       </c>
       <c r="G194" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="195" spans="1:7" x14ac:dyDescent="0.2">
@@ -7194,10 +7191,10 @@
         <v>194</v>
       </c>
       <c r="B195" t="s">
-        <v>277</v>
+        <v>602</v>
       </c>
       <c r="C195" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="D195" s="1">
         <v>69</v>
@@ -7206,10 +7203,10 @@
         <v>1</v>
       </c>
       <c r="F195" t="s">
-        <v>565</v>
+        <v>552</v>
       </c>
       <c r="G195" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="196" spans="1:7" x14ac:dyDescent="0.2">
@@ -7217,10 +7214,10 @@
         <v>195</v>
       </c>
       <c r="B196" t="s">
-        <v>277</v>
+        <v>602</v>
       </c>
       <c r="C196" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="D196" s="1">
         <v>179</v>
@@ -7229,10 +7226,10 @@
         <v>1</v>
       </c>
       <c r="F196" t="s">
-        <v>566</v>
+        <v>553</v>
       </c>
       <c r="G196" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="197" spans="1:7" x14ac:dyDescent="0.2">
@@ -7240,10 +7237,10 @@
         <v>196</v>
       </c>
       <c r="B197" t="s">
-        <v>277</v>
+        <v>602</v>
       </c>
       <c r="C197" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="D197" s="1">
         <v>229</v>
@@ -7252,10 +7249,10 @@
         <v>1</v>
       </c>
       <c r="F197" t="s">
-        <v>567</v>
+        <v>554</v>
       </c>
       <c r="G197" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
     </row>
     <row r="198" spans="1:7" x14ac:dyDescent="0.2">
@@ -7263,10 +7260,10 @@
         <v>197</v>
       </c>
       <c r="B198" t="s">
-        <v>277</v>
+        <v>602</v>
       </c>
       <c r="C198" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="D198" s="1">
         <v>269</v>
@@ -7275,10 +7272,10 @@
         <v>1</v>
       </c>
       <c r="F198" t="s">
-        <v>568</v>
+        <v>555</v>
       </c>
       <c r="G198" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="199" spans="1:7" x14ac:dyDescent="0.2">
@@ -7286,10 +7283,10 @@
         <v>198</v>
       </c>
       <c r="B199" t="s">
-        <v>277</v>
+        <v>602</v>
       </c>
       <c r="C199" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="D199" s="1">
         <v>269</v>
@@ -7298,10 +7295,10 @@
         <v>0</v>
       </c>
       <c r="F199" t="s">
-        <v>569</v>
+        <v>556</v>
       </c>
       <c r="G199" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="200" spans="1:7" x14ac:dyDescent="0.2">
@@ -7309,10 +7306,10 @@
         <v>199</v>
       </c>
       <c r="B200" t="s">
-        <v>277</v>
+        <v>602</v>
       </c>
       <c r="C200" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="D200" s="1">
         <v>399</v>
@@ -7321,10 +7318,10 @@
         <v>1</v>
       </c>
       <c r="F200" t="s">
-        <v>570</v>
+        <v>557</v>
       </c>
       <c r="G200" s="5" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="201" spans="1:7" x14ac:dyDescent="0.2">
@@ -7332,10 +7329,10 @@
         <v>200</v>
       </c>
       <c r="B201" t="s">
-        <v>277</v>
+        <v>602</v>
       </c>
       <c r="C201" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="D201" s="1">
         <v>399</v>
@@ -7344,10 +7341,10 @@
         <v>1</v>
       </c>
       <c r="F201" t="s">
-        <v>571</v>
+        <v>558</v>
       </c>
       <c r="G201" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="202" spans="1:7" x14ac:dyDescent="0.2">
@@ -7355,10 +7352,10 @@
         <v>201</v>
       </c>
       <c r="B202" t="s">
-        <v>277</v>
+        <v>602</v>
       </c>
       <c r="C202" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="D202" s="1">
         <v>599</v>
@@ -7367,10 +7364,10 @@
         <v>1</v>
       </c>
       <c r="F202" t="s">
-        <v>572</v>
+        <v>559</v>
       </c>
       <c r="G202" s="5" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="203" spans="1:7" x14ac:dyDescent="0.2">
@@ -7378,10 +7375,10 @@
         <v>202</v>
       </c>
       <c r="B203" t="s">
-        <v>277</v>
+        <v>602</v>
       </c>
       <c r="C203" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="D203" s="1">
         <v>999</v>
@@ -7390,10 +7387,10 @@
         <v>1</v>
       </c>
       <c r="F203" t="s">
-        <v>573</v>
+        <v>560</v>
       </c>
       <c r="G203" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="204" spans="1:7" x14ac:dyDescent="0.2">
@@ -7401,10 +7398,10 @@
         <v>203</v>
       </c>
       <c r="B204" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="C204" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="D204" s="1">
         <v>5.2</v>
@@ -7413,10 +7410,10 @@
         <v>1</v>
       </c>
       <c r="F204" t="s">
-        <v>574</v>
+        <v>561</v>
       </c>
       <c r="G204" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="205" spans="1:7" x14ac:dyDescent="0.2">
@@ -7424,10 +7421,10 @@
         <v>204</v>
       </c>
       <c r="B205" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="C205" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="D205" s="1">
         <v>7.15</v>
@@ -7436,10 +7433,10 @@
         <v>1</v>
       </c>
       <c r="F205" t="s">
-        <v>574</v>
+        <v>561</v>
       </c>
       <c r="G205" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="206" spans="1:7" x14ac:dyDescent="0.2">
@@ -7447,10 +7444,10 @@
         <v>205</v>
       </c>
       <c r="B206" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="C206" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="D206" s="1">
         <v>12.95</v>
@@ -7459,10 +7456,10 @@
         <v>1</v>
       </c>
       <c r="F206" t="s">
-        <v>575</v>
+        <v>562</v>
       </c>
       <c r="G206" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="207" spans="1:7" x14ac:dyDescent="0.2">
@@ -7470,10 +7467,10 @@
         <v>206</v>
       </c>
       <c r="B207" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="C207" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="D207" s="1">
         <v>16.25</v>
@@ -7482,10 +7479,10 @@
         <v>1</v>
       </c>
       <c r="F207" t="s">
-        <v>574</v>
+        <v>561</v>
       </c>
       <c r="G207" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="208" spans="1:7" x14ac:dyDescent="0.2">
@@ -7493,10 +7490,10 @@
         <v>207</v>
       </c>
       <c r="B208" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="C208" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="D208" s="1">
         <v>25</v>
@@ -7505,10 +7502,10 @@
         <v>1</v>
       </c>
       <c r="F208" t="s">
-        <v>576</v>
+        <v>563</v>
       </c>
       <c r="G208" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="209" spans="1:7" x14ac:dyDescent="0.2">
@@ -7516,10 +7513,10 @@
         <v>208</v>
       </c>
       <c r="B209" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="C209" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="D209" s="1">
         <v>100</v>
@@ -7528,10 +7525,10 @@
         <v>1</v>
       </c>
       <c r="F209" t="s">
-        <v>577</v>
+        <v>564</v>
       </c>
       <c r="G209" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
     <row r="210" spans="1:7" x14ac:dyDescent="0.2">
@@ -7539,10 +7536,10 @@
         <v>209</v>
       </c>
       <c r="B210" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="C210" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="D210" s="1">
         <v>3.9</v>
@@ -7551,10 +7548,10 @@
         <v>1</v>
       </c>
       <c r="F210" t="s">
-        <v>578</v>
+        <v>565</v>
       </c>
       <c r="G210" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
     </row>
     <row r="211" spans="1:7" x14ac:dyDescent="0.2">
@@ -7562,10 +7559,10 @@
         <v>210</v>
       </c>
       <c r="B211" t="s">
+        <v>305</v>
+      </c>
+      <c r="C211" t="s">
         <v>308</v>
-      </c>
-      <c r="C211" t="s">
-        <v>311</v>
       </c>
       <c r="D211" s="1">
         <v>6.9</v>
@@ -7574,10 +7571,10 @@
         <v>1</v>
       </c>
       <c r="F211" t="s">
-        <v>579</v>
+        <v>566</v>
       </c>
       <c r="G211" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
     </row>
     <row r="212" spans="1:7" x14ac:dyDescent="0.2">
@@ -7585,10 +7582,10 @@
         <v>211</v>
       </c>
       <c r="B212" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="C212" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="D212" s="1">
         <v>29</v>
@@ -7597,10 +7594,10 @@
         <v>1</v>
       </c>
       <c r="F212" t="s">
-        <v>580</v>
+        <v>567</v>
       </c>
       <c r="G212" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
     </row>
     <row r="213" spans="1:7" x14ac:dyDescent="0.2">
@@ -7608,10 +7605,10 @@
         <v>212</v>
       </c>
       <c r="B213" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="C213" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="D213" s="1">
         <v>39.9</v>
@@ -7620,10 +7617,10 @@
         <v>1</v>
       </c>
       <c r="F213" t="s">
-        <v>581</v>
+        <v>568</v>
       </c>
       <c r="G213" s="5" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
     </row>
     <row r="214" spans="1:7" x14ac:dyDescent="0.2">
@@ -7631,10 +7628,10 @@
         <v>213</v>
       </c>
       <c r="B214" t="s">
-        <v>315</v>
+        <v>603</v>
       </c>
       <c r="C214" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="D214" s="1">
         <v>7</v>
@@ -7643,10 +7640,10 @@
         <v>1</v>
       </c>
       <c r="F214" t="s">
-        <v>582</v>
+        <v>569</v>
       </c>
       <c r="G214" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
     </row>
     <row r="215" spans="1:7" x14ac:dyDescent="0.2">
@@ -7654,10 +7651,10 @@
         <v>214</v>
       </c>
       <c r="B215" t="s">
-        <v>315</v>
+        <v>603</v>
       </c>
       <c r="C215" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="D215" s="1">
         <v>12.9</v>
@@ -7666,10 +7663,10 @@
         <v>1</v>
       </c>
       <c r="F215" t="s">
-        <v>583</v>
+        <v>570</v>
       </c>
       <c r="G215" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
     </row>
     <row r="216" spans="1:7" x14ac:dyDescent="0.2">
@@ -7677,10 +7674,10 @@
         <v>215</v>
       </c>
       <c r="B216" t="s">
+        <v>603</v>
+      </c>
+      <c r="C216" t="s">
         <v>315</v>
-      </c>
-      <c r="C216" t="s">
-        <v>319</v>
       </c>
       <c r="D216" s="1">
         <v>34.5</v>
@@ -7689,10 +7686,10 @@
         <v>1</v>
       </c>
       <c r="F216" t="s">
-        <v>584</v>
+        <v>571</v>
       </c>
       <c r="G216" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
     </row>
     <row r="217" spans="1:7" x14ac:dyDescent="0.2">
@@ -7700,10 +7697,10 @@
         <v>216</v>
       </c>
       <c r="B217" t="s">
-        <v>315</v>
+        <v>603</v>
       </c>
       <c r="C217" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="D217" s="1">
         <v>99</v>
@@ -7712,10 +7709,10 @@
         <v>1</v>
       </c>
       <c r="F217" t="s">
-        <v>585</v>
+        <v>572</v>
       </c>
       <c r="G217" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
     </row>
     <row r="218" spans="1:7" x14ac:dyDescent="0.2">
@@ -7723,10 +7720,10 @@
         <v>217</v>
       </c>
       <c r="B218" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="C218" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="D218" s="1">
         <v>39</v>
@@ -7735,10 +7732,10 @@
         <v>1</v>
       </c>
       <c r="F218" t="s">
-        <v>586</v>
+        <v>573</v>
       </c>
       <c r="G218" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
     </row>
     <row r="219" spans="1:7" x14ac:dyDescent="0.2">
@@ -7746,10 +7743,10 @@
         <v>218</v>
       </c>
       <c r="B219" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="C219" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="D219" s="1">
         <v>45</v>
@@ -7758,10 +7755,10 @@
         <v>1</v>
       </c>
       <c r="F219" t="s">
-        <v>587</v>
+        <v>574</v>
       </c>
       <c r="G219" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
     </row>
     <row r="220" spans="1:7" x14ac:dyDescent="0.2">
@@ -7769,10 +7766,10 @@
         <v>219</v>
       </c>
       <c r="B220" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="C220" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="D220" s="1">
         <v>100</v>
@@ -7781,10 +7778,10 @@
         <v>1</v>
       </c>
       <c r="F220" t="s">
-        <v>588</v>
+        <v>575</v>
       </c>
       <c r="G220" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
     </row>
     <row r="221" spans="1:7" x14ac:dyDescent="0.2">
@@ -7792,10 +7789,10 @@
         <v>220</v>
       </c>
       <c r="B221" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="C221" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="D221" s="1">
         <v>299</v>
@@ -7804,10 +7801,10 @@
         <v>1</v>
       </c>
       <c r="F221" t="s">
-        <v>589</v>
+        <v>576</v>
       </c>
       <c r="G221" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
     </row>
     <row r="222" spans="1:7" x14ac:dyDescent="0.2">
@@ -7815,10 +7812,10 @@
         <v>221</v>
       </c>
       <c r="B222" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="C222" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="D222" s="1">
         <v>25</v>
@@ -7827,10 +7824,10 @@
         <v>1</v>
       </c>
       <c r="F222" t="s">
-        <v>590</v>
+        <v>577</v>
       </c>
       <c r="G222" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
     </row>
     <row r="223" spans="1:7" x14ac:dyDescent="0.2">
@@ -7838,10 +7835,10 @@
         <v>222</v>
       </c>
       <c r="B223" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="C223" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="D223" s="1">
         <v>25</v>
@@ -7850,10 +7847,10 @@
         <v>1</v>
       </c>
       <c r="F223" t="s">
-        <v>591</v>
+        <v>578</v>
       </c>
       <c r="G223" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
     </row>
     <row r="224" spans="1:7" x14ac:dyDescent="0.2">
@@ -7861,10 +7858,10 @@
         <v>223</v>
       </c>
       <c r="B224" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="C224" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="D224" s="1">
         <v>25</v>
@@ -7873,10 +7870,10 @@
         <v>1</v>
       </c>
       <c r="F224" t="s">
-        <v>592</v>
+        <v>579</v>
       </c>
       <c r="G224" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
     </row>
     <row r="225" spans="1:7" x14ac:dyDescent="0.2">
@@ -7884,10 +7881,10 @@
         <v>224</v>
       </c>
       <c r="B225" t="s">
+        <v>322</v>
+      </c>
+      <c r="C225" t="s">
         <v>326</v>
-      </c>
-      <c r="C225" t="s">
-        <v>330</v>
       </c>
       <c r="D225" s="1">
         <v>25</v>
@@ -7896,10 +7893,10 @@
         <v>1</v>
       </c>
       <c r="F225" t="s">
-        <v>593</v>
+        <v>580</v>
       </c>
       <c r="G225" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
     </row>
     <row r="226" spans="1:7" x14ac:dyDescent="0.2">
@@ -7907,10 +7904,10 @@
         <v>225</v>
       </c>
       <c r="B226" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="C226" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="D226" s="1">
         <v>25</v>
@@ -7919,10 +7916,10 @@
         <v>1</v>
       </c>
       <c r="F226" t="s">
-        <v>594</v>
+        <v>581</v>
       </c>
       <c r="G226" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
     </row>
     <row r="227" spans="1:7" x14ac:dyDescent="0.2">
@@ -7930,10 +7927,10 @@
         <v>226</v>
       </c>
       <c r="B227" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="C227" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="D227" s="1">
         <v>19</v>
@@ -7942,10 +7939,10 @@
         <v>1</v>
       </c>
       <c r="F227" t="s">
-        <v>595</v>
+        <v>582</v>
       </c>
       <c r="G227" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
     </row>
     <row r="228" spans="1:7" x14ac:dyDescent="0.2">
@@ -7953,10 +7950,10 @@
         <v>227</v>
       </c>
       <c r="B228" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="C228" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="D228" s="1">
         <v>19</v>
@@ -7965,10 +7962,10 @@
         <v>1</v>
       </c>
       <c r="F228" t="s">
-        <v>595</v>
+        <v>582</v>
       </c>
       <c r="G228" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
     </row>
     <row r="229" spans="1:7" x14ac:dyDescent="0.2">
@@ -7976,10 +7973,10 @@
         <v>228</v>
       </c>
       <c r="B229" t="s">
+        <v>328</v>
+      </c>
+      <c r="C229" t="s">
         <v>332</v>
-      </c>
-      <c r="C229" t="s">
-        <v>336</v>
       </c>
       <c r="D229" s="1">
         <v>19</v>
@@ -7988,10 +7985,10 @@
         <v>1</v>
       </c>
       <c r="F229" t="s">
-        <v>595</v>
+        <v>582</v>
       </c>
       <c r="G229" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
     </row>
     <row r="230" spans="1:7" x14ac:dyDescent="0.2">
@@ -7999,10 +7996,10 @@
         <v>229</v>
       </c>
       <c r="B230" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="C230" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="D230" s="1">
         <v>19</v>
@@ -8011,10 +8008,10 @@
         <v>1</v>
       </c>
       <c r="F230" t="s">
-        <v>595</v>
+        <v>582</v>
       </c>
       <c r="G230" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
     </row>
     <row r="231" spans="1:7" x14ac:dyDescent="0.2">
@@ -8022,10 +8019,10 @@
         <v>230</v>
       </c>
       <c r="B231" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="C231" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="D231" s="1">
         <v>6</v>
@@ -8034,10 +8031,10 @@
         <v>1</v>
       </c>
       <c r="F231" t="s">
-        <v>596</v>
+        <v>583</v>
       </c>
       <c r="G231" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
     </row>
     <row r="232" spans="1:7" x14ac:dyDescent="0.2">
@@ -8045,10 +8042,10 @@
         <v>231</v>
       </c>
       <c r="B232" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="C232" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="D232" s="1">
         <v>6</v>
@@ -8057,10 +8054,10 @@
         <v>1</v>
       </c>
       <c r="F232" t="s">
-        <v>597</v>
+        <v>584</v>
       </c>
       <c r="G232" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
     </row>
     <row r="233" spans="1:7" x14ac:dyDescent="0.2">
@@ -8068,10 +8065,10 @@
         <v>232</v>
       </c>
       <c r="B233" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="C233" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="D233" s="1">
         <v>9.9</v>
@@ -8080,10 +8077,10 @@
         <v>1</v>
       </c>
       <c r="F233" t="s">
-        <v>598</v>
+        <v>585</v>
       </c>
       <c r="G233" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
     </row>
     <row r="234" spans="1:7" x14ac:dyDescent="0.2">
@@ -8091,10 +8088,10 @@
         <v>233</v>
       </c>
       <c r="B234" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="C234" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="D234" s="1">
         <v>9.9</v>
@@ -8103,10 +8100,10 @@
         <v>1</v>
       </c>
       <c r="F234" t="s">
-        <v>599</v>
+        <v>586</v>
       </c>
       <c r="G234" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
     </row>
     <row r="235" spans="1:7" x14ac:dyDescent="0.2">
@@ -8114,10 +8111,10 @@
         <v>234</v>
       </c>
       <c r="B235" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="C235" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="D235" s="1">
         <v>9.9</v>
@@ -8126,10 +8123,10 @@
         <v>1</v>
       </c>
       <c r="F235" t="s">
-        <v>600</v>
+        <v>587</v>
       </c>
       <c r="G235" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
     </row>
     <row r="236" spans="1:7" x14ac:dyDescent="0.2">
@@ -8137,10 +8134,10 @@
         <v>235</v>
       </c>
       <c r="B236" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="C236" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="D236" s="1">
         <v>9.9</v>
@@ -8149,10 +8146,10 @@
         <v>1</v>
       </c>
       <c r="F236" t="s">
-        <v>601</v>
+        <v>588</v>
       </c>
       <c r="G236" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
     </row>
     <row r="237" spans="1:7" x14ac:dyDescent="0.2">
@@ -8160,10 +8157,10 @@
         <v>236</v>
       </c>
       <c r="B237" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="C237" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="D237" s="1">
         <v>12</v>
@@ -8172,10 +8169,10 @@
         <v>1</v>
       </c>
       <c r="F237" t="s">
-        <v>602</v>
+        <v>589</v>
       </c>
       <c r="G237" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
     </row>
     <row r="238" spans="1:7" x14ac:dyDescent="0.2">
@@ -8183,10 +8180,10 @@
         <v>237</v>
       </c>
       <c r="B238" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="C238" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="D238" s="1">
         <v>18.899999999999999</v>
@@ -8195,10 +8192,10 @@
         <v>1</v>
       </c>
       <c r="F238" t="s">
-        <v>603</v>
+        <v>590</v>
       </c>
       <c r="G238" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
     </row>
     <row r="239" spans="1:7" x14ac:dyDescent="0.2">
@@ -8206,10 +8203,10 @@
         <v>238</v>
       </c>
       <c r="B239" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="C239" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="D239" s="1">
         <v>18.899999999999999</v>
@@ -8218,10 +8215,10 @@
         <v>1</v>
       </c>
       <c r="F239" t="s">
-        <v>604</v>
+        <v>591</v>
       </c>
       <c r="G239" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
     </row>
     <row r="240" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
FIxed real data, changed images to load with long names :)
</commit_message>
<xml_diff>
--- a/cintamani-next/data/products.xlsx
+++ b/cintamani-next/data/products.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-32460" yWindow="2160" windowWidth="23040" windowHeight="9640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2160" windowWidth="23040" windowHeight="9640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="catalog_product_bearbeitet" sheetId="1" r:id="rId1"/>
+    <sheet name="catalog_not_found" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
@@ -1427,9 +1428,6 @@
     <t>MBAva009.JPG</t>
   </si>
   <si>
-    <t>MBAva014.JPG, MBAva015.JPG, MBAva016.JPG, MBAva017.JPG, MBAva018.JPG, MBAva019.JPG</t>
-  </si>
-  <si>
     <t>MBMan008.JPG</t>
   </si>
   <si>
@@ -1817,9 +1815,6 @@
     <t>TBT011.JPG, TBT012.JPG, TBT013.JPG, TBT014.JPG</t>
   </si>
   <si>
-    <t>TBT020.jpg, TBT019.JPG, TBT018.jpg</t>
-  </si>
-  <si>
     <t>TBT021.JPG, TBT022.JPG, TBT023.JPG</t>
   </si>
   <si>
@@ -1845,6 +1840,12 @@
   </si>
   <si>
     <t>weiteres - Räucherzubehör</t>
+  </si>
+  <si>
+    <t>TBT020.JPG, TBT019.JPG, TBT018.JPG</t>
+  </si>
+  <si>
+    <t>MBAva014.JPG, MBAva015.JPG, MBAva016.JPG, MBAva017.JPG, MBAva019.JPG</t>
   </si>
 </sst>
 </file>
@@ -2714,8 +2715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G240"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A206" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D217" sqref="D217"/>
+    <sheetView tabSelected="1" topLeftCell="A231" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A242" sqref="A242"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4886,29 +4887,6 @@
         <v>125</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A95">
-        <v>94</v>
-      </c>
-      <c r="B95" t="s">
-        <v>122</v>
-      </c>
-      <c r="C95" t="s">
-        <v>135</v>
-      </c>
-      <c r="D95" s="1">
-        <v>999</v>
-      </c>
-      <c r="E95">
-        <v>1</v>
-      </c>
-      <c r="F95" t="s">
-        <v>464</v>
-      </c>
-      <c r="G95" t="s">
-        <v>134</v>
-      </c>
-    </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>95</v>
@@ -4926,7 +4904,7 @@
         <v>1</v>
       </c>
       <c r="F96" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="G96" t="s">
         <v>144</v>
@@ -4949,7 +4927,7 @@
         <v>1</v>
       </c>
       <c r="F97" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="G97" t="s">
         <v>359</v>
@@ -4972,7 +4950,7 @@
         <v>1</v>
       </c>
       <c r="F98" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G98" t="s">
         <v>143</v>
@@ -4995,7 +4973,7 @@
         <v>1</v>
       </c>
       <c r="F99" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G99" t="s">
         <v>145</v>
@@ -5018,7 +4996,7 @@
         <v>1</v>
       </c>
       <c r="F100" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="G100" t="s">
         <v>360</v>
@@ -5041,7 +5019,7 @@
         <v>1</v>
       </c>
       <c r="F101" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G101" s="5" t="s">
         <v>141</v>
@@ -5064,7 +5042,7 @@
         <v>1</v>
       </c>
       <c r="F102" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="G102" t="s">
         <v>362</v>
@@ -5087,7 +5065,7 @@
         <v>1</v>
       </c>
       <c r="F103" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="G103" s="5" t="s">
         <v>150</v>
@@ -5110,7 +5088,7 @@
         <v>1</v>
       </c>
       <c r="F104" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="G104" t="s">
         <v>146</v>
@@ -5133,7 +5111,7 @@
         <v>1</v>
       </c>
       <c r="F105" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="G105" s="5" t="s">
         <v>147</v>
@@ -5156,7 +5134,7 @@
         <v>1</v>
       </c>
       <c r="F106" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="G106" t="s">
         <v>170</v>
@@ -5179,7 +5157,7 @@
         <v>1</v>
       </c>
       <c r="F107" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="G107" t="s">
         <v>170</v>
@@ -5202,7 +5180,7 @@
         <v>1</v>
       </c>
       <c r="F108" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="G108" t="s">
         <v>170</v>
@@ -5225,7 +5203,7 @@
         <v>1</v>
       </c>
       <c r="F109" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="G109" t="s">
         <v>170</v>
@@ -5248,7 +5226,7 @@
         <v>1</v>
       </c>
       <c r="F110" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="G110" t="s">
         <v>170</v>
@@ -5271,7 +5249,7 @@
         <v>1</v>
       </c>
       <c r="F111" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="G111" t="s">
         <v>170</v>
@@ -5294,7 +5272,7 @@
         <v>1</v>
       </c>
       <c r="F112" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G112" t="s">
         <v>153</v>
@@ -5317,7 +5295,7 @@
         <v>1</v>
       </c>
       <c r="F113" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="G113" t="s">
         <v>178</v>
@@ -5340,7 +5318,7 @@
         <v>1</v>
       </c>
       <c r="F114" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="G114" t="s">
         <v>165</v>
@@ -5363,7 +5341,7 @@
         <v>1</v>
       </c>
       <c r="F115" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="G115" t="s">
         <v>165</v>
@@ -5386,7 +5364,7 @@
         <v>1</v>
       </c>
       <c r="F116" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="G116" t="s">
         <v>168</v>
@@ -5409,7 +5387,7 @@
         <v>1</v>
       </c>
       <c r="F117" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G117" t="s">
         <v>165</v>
@@ -5432,7 +5410,7 @@
         <v>1</v>
       </c>
       <c r="F118" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G118" t="s">
         <v>155</v>
@@ -5455,7 +5433,7 @@
         <v>1</v>
       </c>
       <c r="F119" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="G119" t="s">
         <v>164</v>
@@ -5478,7 +5456,7 @@
         <v>1</v>
       </c>
       <c r="F120" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="G120" t="s">
         <v>170</v>
@@ -5501,7 +5479,7 @@
         <v>1</v>
       </c>
       <c r="F121" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="G121" t="s">
         <v>170</v>
@@ -5524,7 +5502,7 @@
         <v>1</v>
       </c>
       <c r="F122" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="G122" t="s">
         <v>159</v>
@@ -5547,7 +5525,7 @@
         <v>1</v>
       </c>
       <c r="F123" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="G123" t="s">
         <v>157</v>
@@ -5570,7 +5548,7 @@
         <v>1</v>
       </c>
       <c r="F124" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="G124" t="s">
         <v>161</v>
@@ -5593,7 +5571,7 @@
         <v>1</v>
       </c>
       <c r="F125" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="G125" t="s">
         <v>162</v>
@@ -5616,7 +5594,7 @@
         <v>1</v>
       </c>
       <c r="F126" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="G126" t="s">
         <v>163</v>
@@ -5639,7 +5617,7 @@
         <v>1</v>
       </c>
       <c r="F127" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="G127" t="s">
         <v>180</v>
@@ -5662,7 +5640,7 @@
         <v>1</v>
       </c>
       <c r="F128" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="G128" t="s">
         <v>180</v>
@@ -5685,7 +5663,7 @@
         <v>1</v>
       </c>
       <c r="F129" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="G129" t="s">
         <v>180</v>
@@ -5708,7 +5686,7 @@
         <v>1</v>
       </c>
       <c r="F130" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="G130" t="s">
         <v>180</v>
@@ -5731,7 +5709,7 @@
         <v>1</v>
       </c>
       <c r="F131" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="G131" t="s">
         <v>180</v>
@@ -5754,7 +5732,7 @@
         <v>1</v>
       </c>
       <c r="F132" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="G132" t="s">
         <v>180</v>
@@ -5777,7 +5755,7 @@
         <v>1</v>
       </c>
       <c r="F133" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="G133" t="s">
         <v>201</v>
@@ -5800,7 +5778,7 @@
         <v>1</v>
       </c>
       <c r="F134" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="G134" t="s">
         <v>180</v>
@@ -5823,7 +5801,7 @@
         <v>1</v>
       </c>
       <c r="F135" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="G135" t="s">
         <v>180</v>
@@ -5846,7 +5824,7 @@
         <v>1</v>
       </c>
       <c r="F136" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="G136" t="s">
         <v>180</v>
@@ -5869,7 +5847,7 @@
         <v>1</v>
       </c>
       <c r="F137" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="G137" t="s">
         <v>190</v>
@@ -5892,7 +5870,7 @@
         <v>1</v>
       </c>
       <c r="F138" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="G138" t="s">
         <v>203</v>
@@ -5915,7 +5893,7 @@
         <v>1</v>
       </c>
       <c r="F139" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="G139" t="s">
         <v>180</v>
@@ -5938,7 +5916,7 @@
         <v>1</v>
       </c>
       <c r="F140" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="G140" t="s">
         <v>199</v>
@@ -5961,7 +5939,7 @@
         <v>1</v>
       </c>
       <c r="F141" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="G141" t="s">
         <v>180</v>
@@ -5984,7 +5962,7 @@
         <v>1</v>
       </c>
       <c r="F142" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="G142" t="s">
         <v>180</v>
@@ -6007,7 +5985,7 @@
         <v>1</v>
       </c>
       <c r="F143" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="G143" t="s">
         <v>195</v>
@@ -6030,7 +6008,7 @@
         <v>1</v>
       </c>
       <c r="F144" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="G144" t="s">
         <v>193</v>
@@ -6053,7 +6031,7 @@
         <v>1</v>
       </c>
       <c r="F145" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="G145" t="s">
         <v>193</v>
@@ -6076,7 +6054,7 @@
         <v>1</v>
       </c>
       <c r="F146" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="G146" t="s">
         <v>217</v>
@@ -6087,7 +6065,7 @@
         <v>146</v>
       </c>
       <c r="B147" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="C147" t="s">
         <v>213</v>
@@ -6099,7 +6077,7 @@
         <v>1</v>
       </c>
       <c r="F147" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="G147" t="s">
         <v>212</v>
@@ -6110,7 +6088,7 @@
         <v>147</v>
       </c>
       <c r="B148" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="C148" t="s">
         <v>214</v>
@@ -6122,7 +6100,7 @@
         <v>1</v>
       </c>
       <c r="F148" t="s">
-        <v>594</v>
+        <v>602</v>
       </c>
       <c r="G148" t="s">
         <v>212</v>
@@ -6133,7 +6111,7 @@
         <v>148</v>
       </c>
       <c r="B149" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="C149" t="s">
         <v>215</v>
@@ -6145,7 +6123,7 @@
         <v>1</v>
       </c>
       <c r="F149" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="G149" t="s">
         <v>212</v>
@@ -6156,7 +6134,7 @@
         <v>149</v>
       </c>
       <c r="B150" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="C150" t="s">
         <v>207</v>
@@ -6168,7 +6146,7 @@
         <v>1</v>
       </c>
       <c r="F150" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="G150" t="s">
         <v>206</v>
@@ -6179,7 +6157,7 @@
         <v>150</v>
       </c>
       <c r="B151" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="C151" t="s">
         <v>208</v>
@@ -6191,7 +6169,7 @@
         <v>1</v>
       </c>
       <c r="F151" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="G151" t="s">
         <v>206</v>
@@ -6202,7 +6180,7 @@
         <v>151</v>
       </c>
       <c r="B152" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="C152" t="s">
         <v>209</v>
@@ -6214,7 +6192,7 @@
         <v>1</v>
       </c>
       <c r="F152" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="G152" t="s">
         <v>206</v>
@@ -6225,7 +6203,7 @@
         <v>152</v>
       </c>
       <c r="B153" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="C153" t="s">
         <v>211</v>
@@ -6237,7 +6215,7 @@
         <v>1</v>
       </c>
       <c r="F153" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="G153" t="s">
         <v>210</v>
@@ -6248,7 +6226,7 @@
         <v>153</v>
       </c>
       <c r="B154" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="C154" t="s">
         <v>205</v>
@@ -6260,7 +6238,7 @@
         <v>1</v>
       </c>
       <c r="F154" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="G154" t="s">
         <v>204</v>
@@ -6283,7 +6261,7 @@
         <v>1</v>
       </c>
       <c r="F155" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="G155" t="s">
         <v>219</v>
@@ -6306,7 +6284,7 @@
         <v>1</v>
       </c>
       <c r="F156" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="G156" t="s">
         <v>221</v>
@@ -6329,7 +6307,7 @@
         <v>1</v>
       </c>
       <c r="F157" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="G157" t="s">
         <v>223</v>
@@ -6352,7 +6330,7 @@
         <v>1</v>
       </c>
       <c r="F158" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="G158" t="s">
         <v>225</v>
@@ -6375,7 +6353,7 @@
         <v>1</v>
       </c>
       <c r="F159" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="G159" t="s">
         <v>227</v>
@@ -6398,7 +6376,7 @@
         <v>1</v>
       </c>
       <c r="F160" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="G160" t="s">
         <v>229</v>
@@ -6421,7 +6399,7 @@
         <v>1</v>
       </c>
       <c r="F161" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="G161" t="s">
         <v>231</v>
@@ -6444,7 +6422,7 @@
         <v>1</v>
       </c>
       <c r="F162" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="G162" t="s">
         <v>233</v>
@@ -6467,7 +6445,7 @@
         <v>1</v>
       </c>
       <c r="F163" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="G163" t="s">
         <v>235</v>
@@ -6490,7 +6468,7 @@
         <v>1</v>
       </c>
       <c r="F164" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="G164" t="s">
         <v>238</v>
@@ -6513,7 +6491,7 @@
         <v>1</v>
       </c>
       <c r="F165" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="G165" t="s">
         <v>238</v>
@@ -6536,7 +6514,7 @@
         <v>1</v>
       </c>
       <c r="F166" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="G166" t="s">
         <v>238</v>
@@ -6559,7 +6537,7 @@
         <v>1</v>
       </c>
       <c r="F167" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="G167" t="s">
         <v>242</v>
@@ -6582,7 +6560,7 @@
         <v>1</v>
       </c>
       <c r="F168" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="G168" t="s">
         <v>242</v>
@@ -6605,7 +6583,7 @@
         <v>1</v>
       </c>
       <c r="F169" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="G169" t="s">
         <v>244</v>
@@ -6628,7 +6606,7 @@
         <v>1</v>
       </c>
       <c r="F170" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="G170" t="s">
         <v>246</v>
@@ -6651,7 +6629,7 @@
         <v>1</v>
       </c>
       <c r="F171" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="G171" t="s">
         <v>250</v>
@@ -6674,7 +6652,7 @@
         <v>1</v>
       </c>
       <c r="F172" s="3" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="G172" s="3" t="s">
         <v>250</v>
@@ -6697,7 +6675,7 @@
         <v>1</v>
       </c>
       <c r="F173" s="3" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="G173" s="3" t="s">
         <v>250</v>
@@ -6720,7 +6698,7 @@
         <v>1</v>
       </c>
       <c r="F174" s="3" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="G174" s="3" t="s">
         <v>364</v>
@@ -6743,7 +6721,7 @@
         <v>1</v>
       </c>
       <c r="F175" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="G175" t="s">
         <v>256</v>
@@ -6766,7 +6744,7 @@
         <v>1</v>
       </c>
       <c r="F176" s="3" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="G176" s="3" t="s">
         <v>259</v>
@@ -6789,33 +6767,10 @@
         <v>1</v>
       </c>
       <c r="F177" s="3" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="G177" s="3" t="s">
         <v>260</v>
-      </c>
-    </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A178">
-        <v>177</v>
-      </c>
-      <c r="B178" t="s">
-        <v>249</v>
-      </c>
-      <c r="C178" t="s">
-        <v>255</v>
-      </c>
-      <c r="D178" s="1">
-        <v>999</v>
-      </c>
-      <c r="E178">
-        <v>1</v>
-      </c>
-      <c r="F178" t="s">
-        <v>536</v>
-      </c>
-      <c r="G178" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.2">
@@ -6835,7 +6790,7 @@
         <v>1</v>
       </c>
       <c r="F179" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G179" t="s">
         <v>256</v>
@@ -6881,7 +6836,7 @@
         <v>1</v>
       </c>
       <c r="F181" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="G181" t="s">
         <v>270</v>
@@ -6892,7 +6847,7 @@
         <v>181</v>
       </c>
       <c r="B182" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="C182" t="s">
         <v>265</v>
@@ -6904,7 +6859,7 @@
         <v>1</v>
       </c>
       <c r="F182" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="G182" t="s">
         <v>265</v>
@@ -6915,7 +6870,7 @@
         <v>182</v>
       </c>
       <c r="B183" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="C183" t="s">
         <v>274</v>
@@ -6927,7 +6882,7 @@
         <v>1</v>
       </c>
       <c r="F183" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="G183" t="s">
         <v>274</v>
@@ -6938,7 +6893,7 @@
         <v>183</v>
       </c>
       <c r="B184" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="C184" t="s">
         <v>263</v>
@@ -6950,7 +6905,7 @@
         <v>1</v>
       </c>
       <c r="F184" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="G184" t="s">
         <v>263</v>
@@ -6961,7 +6916,7 @@
         <v>184</v>
       </c>
       <c r="B185" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="C185" t="s">
         <v>273</v>
@@ -6973,7 +6928,7 @@
         <v>1</v>
       </c>
       <c r="F185" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="G185" t="s">
         <v>273</v>
@@ -6984,7 +6939,7 @@
         <v>185</v>
       </c>
       <c r="B186" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="C186" t="s">
         <v>272</v>
@@ -6996,7 +6951,7 @@
         <v>0</v>
       </c>
       <c r="F186" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="G186" t="s">
         <v>271</v>
@@ -7007,7 +6962,7 @@
         <v>186</v>
       </c>
       <c r="B187" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="C187" t="s">
         <v>272</v>
@@ -7019,7 +6974,7 @@
         <v>1</v>
       </c>
       <c r="F187" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="G187" t="s">
         <v>271</v>
@@ -7030,7 +6985,7 @@
         <v>187</v>
       </c>
       <c r="B188" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="C188" t="s">
         <v>264</v>
@@ -7042,7 +6997,7 @@
         <v>1</v>
       </c>
       <c r="F188" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="G188" t="s">
         <v>264</v>
@@ -7053,7 +7008,7 @@
         <v>188</v>
       </c>
       <c r="B189" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="C189" t="s">
         <v>268</v>
@@ -7065,7 +7020,7 @@
         <v>1</v>
       </c>
       <c r="F189" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="G189" s="5" t="s">
         <v>261</v>
@@ -7076,7 +7031,7 @@
         <v>189</v>
       </c>
       <c r="B190" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="C190" t="s">
         <v>267</v>
@@ -7088,7 +7043,7 @@
         <v>1</v>
       </c>
       <c r="F190" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="G190" s="5" t="s">
         <v>266</v>
@@ -7099,7 +7054,7 @@
         <v>190</v>
       </c>
       <c r="B191" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="C191" t="s">
         <v>262</v>
@@ -7111,7 +7066,7 @@
         <v>1</v>
       </c>
       <c r="F191" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="G191" s="5" t="s">
         <v>261</v>
@@ -7122,7 +7077,7 @@
         <v>191</v>
       </c>
       <c r="B192" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="C192" t="s">
         <v>269</v>
@@ -7134,7 +7089,7 @@
         <v>1</v>
       </c>
       <c r="F192" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="G192" t="s">
         <v>269</v>
@@ -7145,7 +7100,7 @@
         <v>192</v>
       </c>
       <c r="B193" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="C193" t="s">
         <v>283</v>
@@ -7157,7 +7112,7 @@
         <v>1</v>
       </c>
       <c r="F193" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="G193" t="s">
         <v>283</v>
@@ -7168,7 +7123,7 @@
         <v>193</v>
       </c>
       <c r="B194" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="C194" t="s">
         <v>281</v>
@@ -7180,7 +7135,7 @@
         <v>1</v>
       </c>
       <c r="F194" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="G194" t="s">
         <v>281</v>
@@ -7191,7 +7146,7 @@
         <v>194</v>
       </c>
       <c r="B195" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="C195" t="s">
         <v>282</v>
@@ -7203,7 +7158,7 @@
         <v>1</v>
       </c>
       <c r="F195" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="G195" t="s">
         <v>282</v>
@@ -7214,7 +7169,7 @@
         <v>195</v>
       </c>
       <c r="B196" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="C196" t="s">
         <v>278</v>
@@ -7226,7 +7181,7 @@
         <v>1</v>
       </c>
       <c r="F196" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="G196" t="s">
         <v>277</v>
@@ -7237,7 +7192,7 @@
         <v>196</v>
       </c>
       <c r="B197" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="C197" t="s">
         <v>285</v>
@@ -7249,7 +7204,7 @@
         <v>1</v>
       </c>
       <c r="F197" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="G197" t="s">
         <v>285</v>
@@ -7260,7 +7215,7 @@
         <v>197</v>
       </c>
       <c r="B198" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="C198" t="s">
         <v>286</v>
@@ -7272,7 +7227,7 @@
         <v>1</v>
       </c>
       <c r="F198" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="G198" t="s">
         <v>286</v>
@@ -7283,7 +7238,7 @@
         <v>198</v>
       </c>
       <c r="B199" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="C199" t="s">
         <v>280</v>
@@ -7295,7 +7250,7 @@
         <v>0</v>
       </c>
       <c r="F199" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="G199" t="s">
         <v>279</v>
@@ -7306,7 +7261,7 @@
         <v>199</v>
       </c>
       <c r="B200" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="C200" t="s">
         <v>276</v>
@@ -7318,7 +7273,7 @@
         <v>1</v>
       </c>
       <c r="F200" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="G200" s="5" t="s">
         <v>275</v>
@@ -7329,7 +7284,7 @@
         <v>200</v>
       </c>
       <c r="B201" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="C201" t="s">
         <v>284</v>
@@ -7341,7 +7296,7 @@
         <v>1</v>
       </c>
       <c r="F201" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="G201" t="s">
         <v>284</v>
@@ -7352,7 +7307,7 @@
         <v>201</v>
       </c>
       <c r="B202" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="C202" t="s">
         <v>288</v>
@@ -7364,7 +7319,7 @@
         <v>1</v>
       </c>
       <c r="F202" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="G202" s="5" t="s">
         <v>287</v>
@@ -7375,7 +7330,7 @@
         <v>202</v>
       </c>
       <c r="B203" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="C203" t="s">
         <v>290</v>
@@ -7387,7 +7342,7 @@
         <v>1</v>
       </c>
       <c r="F203" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="G203" t="s">
         <v>289</v>
@@ -7410,7 +7365,7 @@
         <v>1</v>
       </c>
       <c r="F204" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="G204" t="s">
         <v>295</v>
@@ -7433,7 +7388,7 @@
         <v>1</v>
       </c>
       <c r="F205" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="G205" t="s">
         <v>297</v>
@@ -7456,7 +7411,7 @@
         <v>1</v>
       </c>
       <c r="F206" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="G206" t="s">
         <v>300</v>
@@ -7479,7 +7434,7 @@
         <v>1</v>
       </c>
       <c r="F207" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="G207" t="s">
         <v>293</v>
@@ -7502,7 +7457,7 @@
         <v>1</v>
       </c>
       <c r="F208" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G208" t="s">
         <v>299</v>
@@ -7525,7 +7480,7 @@
         <v>1</v>
       </c>
       <c r="F209" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="G209" t="s">
         <v>303</v>
@@ -7548,7 +7503,7 @@
         <v>1</v>
       </c>
       <c r="F210" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="G210" t="s">
         <v>306</v>
@@ -7571,7 +7526,7 @@
         <v>1</v>
       </c>
       <c r="F211" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="G211" t="s">
         <v>306</v>
@@ -7594,7 +7549,7 @@
         <v>1</v>
       </c>
       <c r="F212" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="G212" t="s">
         <v>306</v>
@@ -7617,7 +7572,7 @@
         <v>1</v>
       </c>
       <c r="F213" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="G213" s="5" t="s">
         <v>310</v>
@@ -7628,7 +7583,7 @@
         <v>213</v>
       </c>
       <c r="B214" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="C214" t="s">
         <v>314</v>
@@ -7640,7 +7595,7 @@
         <v>1</v>
       </c>
       <c r="F214" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="G214" t="s">
         <v>314</v>
@@ -7651,7 +7606,7 @@
         <v>214</v>
       </c>
       <c r="B215" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="C215" t="s">
         <v>313</v>
@@ -7663,7 +7618,7 @@
         <v>1</v>
       </c>
       <c r="F215" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="G215" t="s">
         <v>313</v>
@@ -7674,7 +7629,7 @@
         <v>215</v>
       </c>
       <c r="B216" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="C216" t="s">
         <v>315</v>
@@ -7686,7 +7641,7 @@
         <v>1</v>
       </c>
       <c r="F216" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="G216" t="s">
         <v>315</v>
@@ -7697,7 +7652,7 @@
         <v>216</v>
       </c>
       <c r="B217" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="C217" t="s">
         <v>312</v>
@@ -7709,7 +7664,7 @@
         <v>1</v>
       </c>
       <c r="F217" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="G217" t="s">
         <v>312</v>
@@ -7732,7 +7687,7 @@
         <v>1</v>
       </c>
       <c r="F218" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="G218" t="s">
         <v>354</v>
@@ -7755,7 +7710,7 @@
         <v>1</v>
       </c>
       <c r="F219" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="G219" t="s">
         <v>317</v>
@@ -7778,7 +7733,7 @@
         <v>1</v>
       </c>
       <c r="F220" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="G220" t="s">
         <v>318</v>
@@ -7801,7 +7756,7 @@
         <v>1</v>
       </c>
       <c r="F221" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="G221" t="s">
         <v>320</v>
@@ -7824,7 +7779,7 @@
         <v>1</v>
       </c>
       <c r="F222" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="G222" t="s">
         <v>323</v>
@@ -7847,7 +7802,7 @@
         <v>1</v>
       </c>
       <c r="F223" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="G223" t="s">
         <v>324</v>
@@ -7870,7 +7825,7 @@
         <v>1</v>
       </c>
       <c r="F224" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="G224" t="s">
         <v>325</v>
@@ -7893,7 +7848,7 @@
         <v>1</v>
       </c>
       <c r="F225" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="G225" t="s">
         <v>326</v>
@@ -7916,7 +7871,7 @@
         <v>1</v>
       </c>
       <c r="F226" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="G226" t="s">
         <v>327</v>
@@ -7939,7 +7894,7 @@
         <v>1</v>
       </c>
       <c r="F227" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="G227" t="s">
         <v>329</v>
@@ -7962,7 +7917,7 @@
         <v>1</v>
       </c>
       <c r="F228" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="G228" t="s">
         <v>329</v>
@@ -7985,7 +7940,7 @@
         <v>1</v>
       </c>
       <c r="F229" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="G229" t="s">
         <v>329</v>
@@ -8008,7 +7963,7 @@
         <v>1</v>
       </c>
       <c r="F230" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="G230" t="s">
         <v>329</v>
@@ -8031,7 +7986,7 @@
         <v>1</v>
       </c>
       <c r="F231" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="G231" t="s">
         <v>334</v>
@@ -8054,7 +8009,7 @@
         <v>1</v>
       </c>
       <c r="F232" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="G232" t="s">
         <v>334</v>
@@ -8077,7 +8032,7 @@
         <v>1</v>
       </c>
       <c r="F233" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="G233" t="s">
         <v>338</v>
@@ -8100,7 +8055,7 @@
         <v>1</v>
       </c>
       <c r="F234" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="G234" t="s">
         <v>338</v>
@@ -8123,7 +8078,7 @@
         <v>1</v>
       </c>
       <c r="F235" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="G235" t="s">
         <v>341</v>
@@ -8146,7 +8101,7 @@
         <v>1</v>
       </c>
       <c r="F236" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="G236" t="s">
         <v>338</v>
@@ -8169,7 +8124,7 @@
         <v>1</v>
       </c>
       <c r="F237" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="G237" t="s">
         <v>344</v>
@@ -8192,7 +8147,7 @@
         <v>1</v>
       </c>
       <c r="F238" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="G238" t="s">
         <v>346</v>
@@ -8215,14 +8170,34 @@
         <v>1</v>
       </c>
       <c r="F239" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="G239" t="s">
         <v>348</v>
       </c>
     </row>
     <row r="240" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D240" s="1"/>
+      <c r="A240">
+        <v>94</v>
+      </c>
+      <c r="B240" t="s">
+        <v>122</v>
+      </c>
+      <c r="C240" t="s">
+        <v>135</v>
+      </c>
+      <c r="D240" s="1">
+        <v>999</v>
+      </c>
+      <c r="E240">
+        <v>1</v>
+      </c>
+      <c r="F240" t="s">
+        <v>603</v>
+      </c>
+      <c r="G240" t="s">
+        <v>134</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="A218:G221">
@@ -8230,4 +8205,42 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95993E71-21F0-7C47-9DDC-025999E47ADB}">
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>177</v>
+      </c>
+      <c r="B1" t="s">
+        <v>249</v>
+      </c>
+      <c r="C1" t="s">
+        <v>255</v>
+      </c>
+      <c r="D1" s="1">
+        <v>999</v>
+      </c>
+      <c r="E1">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>535</v>
+      </c>
+      <c r="G1" t="s">
+        <v>254</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>